<commit_message>
fix: modiify some calculate file logic
</commit_message>
<xml_diff>
--- a/成本核算数据源配置表.xlsx
+++ b/成本核算数据源配置表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinliao/Projects/gitclone/python-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{087C5ABD-DC1E-A841-B258-33DC1E4378DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90453F3-3A79-7645-B15D-E3AC95FC8E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-69440" yWindow="-640" windowWidth="28800" windowHeight="17500" xr2:uid="{97E2786A-046E-A540-BAE7-43526A264538}"/>
+    <workbookView xWindow="-69460" yWindow="-640" windowWidth="28800" windowHeight="17500" xr2:uid="{97E2786A-046E-A540-BAE7-43526A264538}"/>
   </bookViews>
   <sheets>
     <sheet name="人员费用配置表" sheetId="1" r:id="rId1"/>
@@ -2415,15 +2415,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2441,6 +2432,24 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2460,53 +2469,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2527,10 +2491,46 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2853,8 +2853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1139A799-FE32-DB46-8CC7-56DA580AFA57}">
   <dimension ref="A1:AL42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AI11" sqref="AI11"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5572,7 +5572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4309A5-7274-AE4A-AEE5-4D23B26A45EE}">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="117" workbookViewId="0">
+    <sheetView zoomScale="117" workbookViewId="0">
       <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
@@ -8582,21 +8582,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="162" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="176" t="s">
+      <c r="B1" s="164" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="176" t="s">
+      <c r="C1" s="164" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="175"/>
-      <c r="B2" s="177"/>
-      <c r="C2" s="177"/>
+      <c r="A2" s="163"/>
+      <c r="B2" s="165"/>
+      <c r="C2" s="165"/>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4">
@@ -8614,7 +8614,7 @@
       <c r="B4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="178"/>
+      <c r="C4" s="166"/>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4">
@@ -8624,7 +8624,7 @@
       <c r="B5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="179"/>
+      <c r="C5" s="167"/>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4">
@@ -8639,18 +8639,18 @@
       <c r="A7" s="168" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="165" t="s">
+      <c r="B7" s="170" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="180" t="s">
+      <c r="C7" s="172" t="s">
         <v>38</v>
       </c>
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="170"/>
-      <c r="B8" s="167"/>
-      <c r="C8" s="181"/>
+      <c r="A8" s="169"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" ht="30">
@@ -8749,24 +8749,24 @@
       <c r="A20" s="168" t="s">
         <v>248</v>
       </c>
-      <c r="B20" s="165" t="s">
+      <c r="B20" s="170" t="s">
         <v>249</v>
       </c>
-      <c r="C20" s="171" t="s">
+      <c r="C20" s="179" t="s">
         <v>254</v>
       </c>
       <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="169"/>
-      <c r="B21" s="166"/>
-      <c r="C21" s="172"/>
+      <c r="A21" s="178"/>
+      <c r="B21" s="177"/>
+      <c r="C21" s="180"/>
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="68" customHeight="1">
-      <c r="A22" s="170"/>
-      <c r="B22" s="167"/>
-      <c r="C22" s="173"/>
+      <c r="A22" s="169"/>
+      <c r="B22" s="171"/>
+      <c r="C22" s="181"/>
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4">
@@ -8802,57 +8802,57 @@
       <c r="D25" s="18"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="162" t="s">
+      <c r="A26" s="174" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="165" t="s">
+      <c r="B26" s="170" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="165" t="s">
+      <c r="C26" s="170" t="s">
         <v>67</v>
       </c>
       <c r="D26" s="18"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="163"/>
-      <c r="B27" s="166"/>
-      <c r="C27" s="166"/>
+      <c r="A27" s="175"/>
+      <c r="B27" s="177"/>
+      <c r="C27" s="177"/>
       <c r="D27" s="15"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="163"/>
-      <c r="B28" s="166"/>
-      <c r="C28" s="166"/>
+      <c r="A28" s="175"/>
+      <c r="B28" s="177"/>
+      <c r="C28" s="177"/>
       <c r="D28" s="18"/>
     </row>
     <row r="29" spans="1:4" ht="40" customHeight="1">
-      <c r="A29" s="164"/>
-      <c r="B29" s="167"/>
-      <c r="C29" s="167"/>
+      <c r="A29" s="176"/>
+      <c r="B29" s="171"/>
+      <c r="C29" s="171"/>
       <c r="D29" s="18"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="162" t="s">
+      <c r="A30" s="174" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="165" t="s">
+      <c r="B30" s="170" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="165" t="s">
+      <c r="C30" s="170" t="s">
         <v>69</v>
       </c>
       <c r="D30" s="18"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="163"/>
-      <c r="B31" s="166"/>
-      <c r="C31" s="166"/>
+      <c r="A31" s="175"/>
+      <c r="B31" s="177"/>
+      <c r="C31" s="177"/>
       <c r="D31" s="18"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="164"/>
-      <c r="B32" s="167"/>
-      <c r="C32" s="167"/>
+      <c r="A32" s="176"/>
+      <c r="B32" s="171"/>
+      <c r="C32" s="171"/>
       <c r="D32" s="18"/>
     </row>
     <row r="33" spans="1:4">
@@ -8873,13 +8873,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
     <mergeCell ref="A30:A32"/>
     <mergeCell ref="B30:B32"/>
     <mergeCell ref="C30:C32"/>
@@ -8889,6 +8882,13 @@
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="C26:C29"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8930,20 +8930,20 @@
       <c r="D1" s="141" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="145" t="s">
+      <c r="E1" s="151" t="s">
         <v>200</v>
       </c>
-      <c r="F1" s="143"/>
-      <c r="G1" s="143"/>
-      <c r="H1" s="143"/>
-      <c r="I1" s="144"/>
+      <c r="F1" s="149"/>
+      <c r="G1" s="149"/>
+      <c r="H1" s="149"/>
+      <c r="I1" s="150"/>
       <c r="J1" s="72" t="s">
         <v>201</v>
       </c>
-      <c r="K1" s="143" t="s">
+      <c r="K1" s="149" t="s">
         <v>240</v>
       </c>
-      <c r="L1" s="144"/>
+      <c r="L1" s="150"/>
     </row>
     <row r="2" spans="1:12" s="15" customFormat="1" ht="68">
       <c r="A2" s="138"/>
@@ -8982,10 +8982,10 @@
       <c r="B3" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="146" t="s">
+      <c r="C3" s="143" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="149" t="s">
+      <c r="D3" s="146" t="s">
         <v>50</v>
       </c>
       <c r="E3" s="67">
@@ -9014,8 +9014,8 @@
       <c r="B4" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="147"/>
-      <c r="D4" s="150"/>
+      <c r="C4" s="144"/>
+      <c r="D4" s="147"/>
       <c r="E4" s="68">
         <v>1</v>
       </c>
@@ -9042,8 +9042,8 @@
       <c r="B5" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="147"/>
-      <c r="D5" s="150"/>
+      <c r="C5" s="144"/>
+      <c r="D5" s="147"/>
       <c r="E5" s="68">
         <v>1</v>
       </c>
@@ -9070,8 +9070,8 @@
       <c r="B6" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="147"/>
-      <c r="D6" s="150"/>
+      <c r="C6" s="144"/>
+      <c r="D6" s="147"/>
       <c r="E6" s="68">
         <v>1</v>
       </c>
@@ -9098,8 +9098,8 @@
       <c r="B7" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="147"/>
-      <c r="D7" s="150"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="147"/>
       <c r="E7" s="68">
         <v>1</v>
       </c>
@@ -9126,8 +9126,8 @@
       <c r="B8" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="147"/>
-      <c r="D8" s="150"/>
+      <c r="C8" s="144"/>
+      <c r="D8" s="147"/>
       <c r="E8" s="68">
         <v>1</v>
       </c>
@@ -9154,8 +9154,8 @@
       <c r="B9" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="147"/>
-      <c r="D9" s="150"/>
+      <c r="C9" s="144"/>
+      <c r="D9" s="147"/>
       <c r="E9" s="68">
         <v>1</v>
       </c>
@@ -9182,8 +9182,8 @@
       <c r="B10" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="147"/>
-      <c r="D10" s="150"/>
+      <c r="C10" s="144"/>
+      <c r="D10" s="147"/>
       <c r="E10" s="68">
         <v>1</v>
       </c>
@@ -9210,8 +9210,8 @@
       <c r="B11" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="147"/>
-      <c r="D11" s="150"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="147"/>
       <c r="E11" s="68">
         <v>1</v>
       </c>
@@ -9238,8 +9238,8 @@
       <c r="B12" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="C12" s="147"/>
-      <c r="D12" s="150"/>
+      <c r="C12" s="144"/>
+      <c r="D12" s="147"/>
       <c r="E12" s="68">
         <v>1</v>
       </c>
@@ -9260,8 +9260,8 @@
       <c r="B13" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="C13" s="147"/>
-      <c r="D13" s="150"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="147"/>
       <c r="E13" s="68">
         <v>1</v>
       </c>
@@ -9280,8 +9280,8 @@
       <c r="B14" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="C14" s="147"/>
-      <c r="D14" s="150"/>
+      <c r="C14" s="144"/>
+      <c r="D14" s="147"/>
       <c r="E14" s="68">
         <v>1</v>
       </c>
@@ -9300,8 +9300,8 @@
       <c r="B15" s="71" t="s">
         <v>194</v>
       </c>
-      <c r="C15" s="147"/>
-      <c r="D15" s="150"/>
+      <c r="C15" s="144"/>
+      <c r="D15" s="147"/>
       <c r="E15" s="68">
         <v>1</v>
       </c>
@@ -9320,8 +9320,8 @@
       <c r="B16" s="85" t="s">
         <v>194</v>
       </c>
-      <c r="C16" s="148"/>
-      <c r="D16" s="151"/>
+      <c r="C16" s="145"/>
+      <c r="D16" s="148"/>
       <c r="E16" s="69">
         <v>1</v>
       </c>
@@ -9340,10 +9340,10 @@
       <c r="B17" s="75" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="146" t="s">
+      <c r="C17" s="143" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="149" t="s">
+      <c r="D17" s="146" t="s">
         <v>50</v>
       </c>
       <c r="E17" s="67">
@@ -9370,8 +9370,8 @@
       <c r="B18" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="C18" s="147"/>
-      <c r="D18" s="150"/>
+      <c r="C18" s="144"/>
+      <c r="D18" s="147"/>
       <c r="E18" s="68">
         <v>1</v>
       </c>
@@ -9396,8 +9396,8 @@
       <c r="B19" s="71" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="147"/>
-      <c r="D19" s="150"/>
+      <c r="C19" s="144"/>
+      <c r="D19" s="147"/>
       <c r="E19" s="68">
         <v>1</v>
       </c>
@@ -9416,8 +9416,8 @@
       <c r="B20" s="71" t="s">
         <v>196</v>
       </c>
-      <c r="C20" s="147"/>
-      <c r="D20" s="150"/>
+      <c r="C20" s="144"/>
+      <c r="D20" s="147"/>
       <c r="E20" s="88">
         <v>1</v>
       </c>
@@ -9436,10 +9436,10 @@
       <c r="B21" s="71" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="147" t="s">
+      <c r="C21" s="144" t="s">
         <v>48</v>
       </c>
-      <c r="D21" s="150" t="s">
+      <c r="D21" s="147" t="s">
         <v>51</v>
       </c>
       <c r="E21" s="68"/>
@@ -9464,8 +9464,8 @@
       <c r="B22" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="147"/>
-      <c r="D22" s="150"/>
+      <c r="C22" s="144"/>
+      <c r="D22" s="147"/>
       <c r="E22" s="68"/>
       <c r="F22" s="62"/>
       <c r="G22" s="62">
@@ -9488,8 +9488,8 @@
       <c r="B23" s="71" t="s">
         <v>76</v>
       </c>
-      <c r="C23" s="147"/>
-      <c r="D23" s="150"/>
+      <c r="C23" s="144"/>
+      <c r="D23" s="147"/>
       <c r="E23" s="68"/>
       <c r="F23" s="62"/>
       <c r="G23" s="62">
@@ -9512,8 +9512,8 @@
       <c r="B24" s="71" t="s">
         <v>239</v>
       </c>
-      <c r="C24" s="147"/>
-      <c r="D24" s="150"/>
+      <c r="C24" s="144"/>
+      <c r="D24" s="147"/>
       <c r="E24" s="68"/>
       <c r="F24" s="62"/>
       <c r="G24" s="62"/>
@@ -9534,8 +9534,8 @@
       <c r="B25" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="C25" s="147"/>
-      <c r="D25" s="150"/>
+      <c r="C25" s="144"/>
+      <c r="D25" s="147"/>
       <c r="E25" s="68"/>
       <c r="F25" s="62"/>
       <c r="G25" s="62"/>
@@ -9556,8 +9556,8 @@
       <c r="B26" s="71" t="s">
         <v>195</v>
       </c>
-      <c r="C26" s="147"/>
-      <c r="D26" s="150"/>
+      <c r="C26" s="144"/>
+      <c r="D26" s="147"/>
       <c r="E26" s="68"/>
       <c r="F26" s="62"/>
       <c r="G26" s="62"/>
@@ -9578,8 +9578,8 @@
       <c r="B27" s="85" t="s">
         <v>195</v>
       </c>
-      <c r="C27" s="148"/>
-      <c r="D27" s="151"/>
+      <c r="C27" s="145"/>
+      <c r="D27" s="148"/>
       <c r="E27" s="69"/>
       <c r="F27" s="64"/>
       <c r="G27" s="64"/>
@@ -9595,18 +9595,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="E1:I1"/>
     <mergeCell ref="C3:C16"/>
     <mergeCell ref="C21:C27"/>
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="D3:D16"/>
     <mergeCell ref="D21:D27"/>
     <mergeCell ref="D17:D20"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="E1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11018,15 +11018,15 @@
       <c r="AD34" s="102"/>
     </row>
     <row r="35" spans="1:30">
-      <c r="A35" s="155" t="s">
+      <c r="A35" s="158" t="s">
         <v>248</v>
       </c>
-      <c r="B35" s="155" t="s">
+      <c r="B35" s="158" t="s">
         <v>367</v>
       </c>
-      <c r="C35" s="155"/>
-      <c r="D35" s="158"/>
-      <c r="E35" s="158"/>
+      <c r="C35" s="158"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="152"/>
       <c r="F35" s="99"/>
       <c r="G35" s="102"/>
       <c r="H35" s="102"/>
@@ -11054,11 +11054,11 @@
       <c r="AD35" s="102"/>
     </row>
     <row r="36" spans="1:30">
-      <c r="A36" s="156"/>
-      <c r="B36" s="156"/>
-      <c r="C36" s="156"/>
-      <c r="D36" s="159"/>
-      <c r="E36" s="159"/>
+      <c r="A36" s="159"/>
+      <c r="B36" s="159"/>
+      <c r="C36" s="159"/>
+      <c r="D36" s="153"/>
+      <c r="E36" s="153"/>
       <c r="F36" s="99"/>
       <c r="G36" s="102"/>
       <c r="H36" s="102"/>
@@ -11086,11 +11086,11 @@
       <c r="AD36" s="102"/>
     </row>
     <row r="37" spans="1:30">
-      <c r="A37" s="157"/>
-      <c r="B37" s="157"/>
-      <c r="C37" s="157"/>
-      <c r="D37" s="160"/>
-      <c r="E37" s="160"/>
+      <c r="A37" s="160"/>
+      <c r="B37" s="160"/>
+      <c r="C37" s="160"/>
+      <c r="D37" s="154"/>
+      <c r="E37" s="154"/>
       <c r="F37" s="99"/>
       <c r="G37" s="102"/>
       <c r="H37" s="102"/>
@@ -11784,15 +11784,15 @@
       <c r="AD54" s="102"/>
     </row>
     <row r="55" spans="1:30">
-      <c r="A55" s="152" t="s">
+      <c r="A55" s="155" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="155" t="s">
+      <c r="B55" s="158" t="s">
         <v>372</v>
       </c>
-      <c r="C55" s="155"/>
-      <c r="D55" s="158"/>
-      <c r="E55" s="158"/>
+      <c r="C55" s="158"/>
+      <c r="D55" s="152"/>
+      <c r="E55" s="152"/>
       <c r="F55" s="112"/>
       <c r="G55" s="102"/>
       <c r="H55" s="102"/>
@@ -11820,11 +11820,11 @@
       <c r="AD55" s="102"/>
     </row>
     <row r="56" spans="1:30">
-      <c r="A56" s="153"/>
-      <c r="B56" s="156"/>
-      <c r="C56" s="156"/>
-      <c r="D56" s="159"/>
-      <c r="E56" s="159"/>
+      <c r="A56" s="156"/>
+      <c r="B56" s="159"/>
+      <c r="C56" s="159"/>
+      <c r="D56" s="153"/>
+      <c r="E56" s="153"/>
       <c r="F56" s="102"/>
       <c r="G56" s="102"/>
       <c r="H56" s="102"/>
@@ -11852,11 +11852,11 @@
       <c r="AD56" s="102"/>
     </row>
     <row r="57" spans="1:30">
-      <c r="A57" s="153"/>
-      <c r="B57" s="156"/>
-      <c r="C57" s="156"/>
-      <c r="D57" s="159"/>
-      <c r="E57" s="159"/>
+      <c r="A57" s="156"/>
+      <c r="B57" s="159"/>
+      <c r="C57" s="159"/>
+      <c r="D57" s="153"/>
+      <c r="E57" s="153"/>
       <c r="F57" s="112"/>
       <c r="G57" s="102"/>
       <c r="H57" s="102"/>
@@ -11884,11 +11884,11 @@
       <c r="AD57" s="102"/>
     </row>
     <row r="58" spans="1:30">
-      <c r="A58" s="154"/>
-      <c r="B58" s="157"/>
-      <c r="C58" s="157"/>
-      <c r="D58" s="160"/>
-      <c r="E58" s="160"/>
+      <c r="A58" s="157"/>
+      <c r="B58" s="160"/>
+      <c r="C58" s="160"/>
+      <c r="D58" s="154"/>
+      <c r="E58" s="154"/>
       <c r="F58" s="112"/>
       <c r="G58" s="102"/>
       <c r="H58" s="102"/>
@@ -12156,15 +12156,15 @@
       <c r="AD64" s="102"/>
     </row>
     <row r="65" spans="1:30" s="44" customFormat="1">
-      <c r="A65" s="152" t="s">
+      <c r="A65" s="155" t="s">
         <v>32</v>
       </c>
-      <c r="B65" s="155" t="s">
+      <c r="B65" s="158" t="s">
         <v>376</v>
       </c>
-      <c r="C65" s="155"/>
-      <c r="D65" s="158"/>
-      <c r="E65" s="158"/>
+      <c r="C65" s="158"/>
+      <c r="D65" s="152"/>
+      <c r="E65" s="152"/>
       <c r="F65" s="112"/>
       <c r="G65" s="102"/>
       <c r="H65" s="102"/>
@@ -12192,11 +12192,11 @@
       <c r="AD65" s="102"/>
     </row>
     <row r="66" spans="1:30" s="44" customFormat="1">
-      <c r="A66" s="153"/>
-      <c r="B66" s="156"/>
-      <c r="C66" s="156"/>
-      <c r="D66" s="159"/>
-      <c r="E66" s="159"/>
+      <c r="A66" s="156"/>
+      <c r="B66" s="159"/>
+      <c r="C66" s="159"/>
+      <c r="D66" s="153"/>
+      <c r="E66" s="153"/>
       <c r="F66" s="112"/>
       <c r="G66" s="102"/>
       <c r="H66" s="102"/>
@@ -12224,11 +12224,11 @@
       <c r="AD66" s="102"/>
     </row>
     <row r="67" spans="1:30">
-      <c r="A67" s="154"/>
-      <c r="B67" s="157"/>
-      <c r="C67" s="157"/>
-      <c r="D67" s="160"/>
-      <c r="E67" s="160"/>
+      <c r="A67" s="157"/>
+      <c r="B67" s="160"/>
+      <c r="C67" s="160"/>
+      <c r="D67" s="154"/>
+      <c r="E67" s="154"/>
       <c r="F67" s="112"/>
       <c r="G67" s="102"/>
       <c r="H67" s="102"/>
@@ -12325,12 +12325,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
     <mergeCell ref="A65:A67"/>
     <mergeCell ref="B65:B67"/>
     <mergeCell ref="C65:C67"/>
@@ -12340,6 +12334,12 @@
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="B55:B58"/>
     <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="D55:D58"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12351,7 +12351,7 @@
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
fix: modify code relation file
</commit_message>
<xml_diff>
--- a/成本核算数据源配置表.xlsx
+++ b/成本核算数据源配置表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinliao/Projects/gitclone/python-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90453F3-3A79-7645-B15D-E3AC95FC8E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BDB724D-6D3B-3F40-8199-9E86FC0725B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-69460" yWindow="-640" windowWidth="28800" windowHeight="17500" xr2:uid="{97E2786A-046E-A540-BAE7-43526A264538}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{97E2786A-046E-A540-BAE7-43526A264538}"/>
   </bookViews>
   <sheets>
     <sheet name="人员费用配置表" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1186" uniqueCount="422">
   <si>
     <t>人员</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1631,6 +1631,10 @@
   </si>
   <si>
     <t>分摊市场人员费用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>研发人员工资  = 工资表[工资] * 人员配置[工资]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2853,8 +2857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1139A799-FE32-DB46-8CC7-56DA580AFA57}">
   <dimension ref="A1:AL42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N2" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8900,7 +8904,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9617,8 +9621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90D46437-804D-5248-B470-EF765C941C69}">
   <dimension ref="A1:AD69"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9626,8 +9630,8 @@
     <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41.1640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.6640625" style="47" customWidth="1"/>
+    <col min="5" max="5" width="52.83203125" style="47" customWidth="1"/>
     <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="9.5" bestFit="1" customWidth="1"/>
@@ -10392,7 +10396,9 @@
         <v>339</v>
       </c>
       <c r="D19" s="98"/>
-      <c r="E19" s="98"/>
+      <c r="E19" s="98" t="s">
+        <v>421</v>
+      </c>
       <c r="F19" s="102"/>
       <c r="G19" s="102"/>
       <c r="H19" s="102"/>
@@ -15957,7 +15963,7 @@
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="P1" sqref="P1:P1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -17768,7 +17774,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
feat: add source data import finance database
</commit_message>
<xml_diff>
--- a/成本核算数据源配置表.xlsx
+++ b/成本核算数据源配置表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinliao/Projects/gitclone/python-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE57C08-B012-944C-A962-9CED729C7727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6F592C-8CF3-C342-B517-0AD6606EBBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68940" yWindow="-820" windowWidth="28800" windowHeight="17500" xr2:uid="{97E2786A-046E-A540-BAE7-43526A264538}"/>
+    <workbookView xWindow="-68940" yWindow="-820" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{97E2786A-046E-A540-BAE7-43526A264538}"/>
   </bookViews>
   <sheets>
     <sheet name="人员费用配置表" sheetId="20" r:id="rId1"/>
@@ -2171,6 +2171,32 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2198,15 +2224,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2215,6 +2232,24 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2234,43 +2269,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="16" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2594,8 +2594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC9293E-C443-5D4F-807A-3A2F963837CD}">
   <dimension ref="A1:BO42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -2604,7 +2604,7 @@
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
     <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
@@ -2616,7 +2616,7 @@
     <col min="16" max="16" width="18.33203125" customWidth="1"/>
     <col min="17" max="19" width="17.6640625" customWidth="1"/>
     <col min="20" max="20" width="16.6640625" customWidth="1"/>
-    <col min="21" max="21" width="6.83203125" style="118" customWidth="1"/>
+    <col min="21" max="21" width="6.83203125" style="93" customWidth="1"/>
     <col min="22" max="30" width="6.83203125" customWidth="1"/>
     <col min="31" max="31" width="18.33203125" customWidth="1"/>
     <col min="32" max="32" width="16" customWidth="1"/>
@@ -2638,107 +2638,107 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="49" customHeight="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="101" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="92" t="s">
+      <c r="C1" s="101" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="92" t="s">
+      <c r="D1" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="92" t="s">
+      <c r="E1" s="101" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="94" t="s">
+      <c r="F1" s="103" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="87" t="s">
+      <c r="G1" s="96" t="s">
         <v>293</v>
       </c>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="87" t="s">
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="96" t="s">
         <v>294</v>
       </c>
-      <c r="O1" s="88"/>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="88" t="s">
+      <c r="O1" s="97"/>
+      <c r="P1" s="97"/>
+      <c r="Q1" s="97"/>
+      <c r="R1" s="97"/>
+      <c r="S1" s="97"/>
+      <c r="T1" s="98"/>
+      <c r="U1" s="97" t="s">
         <v>399</v>
       </c>
-      <c r="V1" s="88"/>
-      <c r="W1" s="88"/>
-      <c r="X1" s="88"/>
-      <c r="Y1" s="88"/>
-      <c r="Z1" s="88"/>
-      <c r="AA1" s="88"/>
-      <c r="AB1" s="88"/>
-      <c r="AC1" s="88"/>
-      <c r="AD1" s="88"/>
-      <c r="AE1" s="88"/>
-      <c r="AF1" s="88"/>
-      <c r="AG1" s="88"/>
-      <c r="AH1" s="88"/>
-      <c r="AI1" s="88"/>
-      <c r="AJ1" s="88"/>
-      <c r="AK1" s="88"/>
-      <c r="AL1" s="87" t="s">
+      <c r="V1" s="97"/>
+      <c r="W1" s="97"/>
+      <c r="X1" s="97"/>
+      <c r="Y1" s="97"/>
+      <c r="Z1" s="97"/>
+      <c r="AA1" s="97"/>
+      <c r="AB1" s="97"/>
+      <c r="AC1" s="97"/>
+      <c r="AD1" s="97"/>
+      <c r="AE1" s="97"/>
+      <c r="AF1" s="97"/>
+      <c r="AG1" s="97"/>
+      <c r="AH1" s="97"/>
+      <c r="AI1" s="97"/>
+      <c r="AJ1" s="97"/>
+      <c r="AK1" s="97"/>
+      <c r="AL1" s="96" t="s">
         <v>400</v>
       </c>
-      <c r="AM1" s="88"/>
-      <c r="AN1" s="88"/>
-      <c r="AO1" s="88"/>
-      <c r="AP1" s="88"/>
-      <c r="AQ1" s="88"/>
-      <c r="AR1" s="89"/>
-      <c r="AS1" s="87" t="s">
+      <c r="AM1" s="97"/>
+      <c r="AN1" s="97"/>
+      <c r="AO1" s="97"/>
+      <c r="AP1" s="97"/>
+      <c r="AQ1" s="97"/>
+      <c r="AR1" s="98"/>
+      <c r="AS1" s="96" t="s">
         <v>295</v>
       </c>
-      <c r="AT1" s="88"/>
-      <c r="AU1" s="88"/>
-      <c r="AV1" s="88"/>
-      <c r="AW1" s="88"/>
-      <c r="AX1" s="88"/>
-      <c r="AY1" s="88"/>
-      <c r="AZ1" s="89"/>
-      <c r="BA1" s="88" t="s">
+      <c r="AT1" s="97"/>
+      <c r="AU1" s="97"/>
+      <c r="AV1" s="97"/>
+      <c r="AW1" s="97"/>
+      <c r="AX1" s="97"/>
+      <c r="AY1" s="97"/>
+      <c r="AZ1" s="98"/>
+      <c r="BA1" s="97" t="s">
         <v>296</v>
       </c>
-      <c r="BB1" s="88"/>
-      <c r="BC1" s="89"/>
-      <c r="BD1" s="87" t="s">
+      <c r="BB1" s="97"/>
+      <c r="BC1" s="98"/>
+      <c r="BD1" s="96" t="s">
         <v>297</v>
       </c>
-      <c r="BE1" s="88"/>
-      <c r="BF1" s="88"/>
-      <c r="BG1" s="88"/>
-      <c r="BH1" s="88"/>
-      <c r="BI1" s="88"/>
-      <c r="BJ1" s="88"/>
-      <c r="BK1" s="88"/>
-      <c r="BL1" s="88"/>
-      <c r="BM1" s="88"/>
-      <c r="BN1" s="88"/>
-      <c r="BO1" s="89"/>
+      <c r="BE1" s="97"/>
+      <c r="BF1" s="97"/>
+      <c r="BG1" s="97"/>
+      <c r="BH1" s="97"/>
+      <c r="BI1" s="97"/>
+      <c r="BJ1" s="97"/>
+      <c r="BK1" s="97"/>
+      <c r="BL1" s="97"/>
+      <c r="BM1" s="97"/>
+      <c r="BN1" s="97"/>
+      <c r="BO1" s="98"/>
     </row>
     <row r="2" spans="1:67" s="1" customFormat="1" ht="68">
-      <c r="A2" s="91"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="95"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="104"/>
       <c r="G2" s="22" t="s">
         <v>298</v>
       </c>
@@ -3080,13 +3080,13 @@
       <c r="AZ3" s="14" t="s">
         <v>360</v>
       </c>
-      <c r="BA3" s="113" t="s">
+      <c r="BA3" s="88" t="s">
         <v>361</v>
       </c>
-      <c r="BB3" s="114" t="s">
+      <c r="BB3" s="89" t="s">
         <v>362</v>
       </c>
-      <c r="BC3" s="115" t="s">
+      <c r="BC3" s="90" t="s">
         <v>363</v>
       </c>
       <c r="BD3" s="23" t="s">
@@ -4577,7 +4577,7 @@
       <c r="AY18" s="11"/>
       <c r="AZ18" s="17"/>
       <c r="BA18" s="11"/>
-      <c r="BB18" s="119"/>
+      <c r="BB18" s="94"/>
       <c r="BC18" s="17"/>
       <c r="BD18" s="26"/>
       <c r="BE18" s="11"/>
@@ -4676,7 +4676,7 @@
       <c r="BA19" s="4">
         <v>1</v>
       </c>
-      <c r="BB19" s="120"/>
+      <c r="BB19" s="95"/>
       <c r="BC19" s="15"/>
       <c r="BD19" s="22"/>
       <c r="BE19" s="4"/>
@@ -4775,7 +4775,7 @@
       <c r="AY20" s="4"/>
       <c r="AZ20" s="15"/>
       <c r="BA20" s="4"/>
-      <c r="BB20" s="120"/>
+      <c r="BB20" s="95"/>
       <c r="BC20" s="15"/>
       <c r="BD20" s="22"/>
       <c r="BE20" s="4"/>
@@ -4874,7 +4874,7 @@
       <c r="BA21" s="4">
         <v>1</v>
       </c>
-      <c r="BB21" s="120"/>
+      <c r="BB21" s="95"/>
       <c r="BC21" s="15"/>
       <c r="BD21" s="22"/>
       <c r="BE21" s="4"/>
@@ -6598,6 +6598,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="BD1:BO1"/>
     <mergeCell ref="G1:M1"/>
     <mergeCell ref="N1:T1"/>
@@ -6605,12 +6611,6 @@
     <mergeCell ref="AL1:AR1"/>
     <mergeCell ref="AS1:AZ1"/>
     <mergeCell ref="BA1:BC1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6621,273 +6621,273 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4309A5-7274-AE4A-AEE5-4D23B26A45EE}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" zoomScale="117" workbookViewId="0">
+    <sheetView zoomScale="117" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:3" ht="17">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="91" t="s">
         <v>376</v>
       </c>
-      <c r="B1" s="116" t="s">
+      <c r="B1" s="91" t="s">
         <v>377</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="C1" s="91" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="117" t="s">
+      <c r="A2" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="117">
+      <c r="C2" s="92">
         <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="117" t="s">
+      <c r="A3" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B3" s="117" t="s">
+      <c r="B3" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="117">
+      <c r="C3" s="92">
         <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="117" t="s">
+      <c r="A4" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="117">
+      <c r="C4" s="92">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="117" t="s">
+      <c r="A5" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="117">
+      <c r="C5" s="92">
         <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="117" t="s">
+      <c r="A6" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="92" t="s">
         <v>380</v>
       </c>
-      <c r="C6" s="117">
+      <c r="C6" s="92">
         <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="92" t="s">
         <v>381</v>
       </c>
-      <c r="C7" s="117">
+      <c r="C7" s="92">
         <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B8" s="117" t="s">
+      <c r="B8" s="92" t="s">
         <v>382</v>
       </c>
-      <c r="C8" s="117">
+      <c r="C8" s="92">
         <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" s="117" t="s">
+      <c r="A9" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B9" s="117" t="s">
+      <c r="B9" s="92" t="s">
         <v>383</v>
       </c>
-      <c r="C9" s="117">
+      <c r="C9" s="92">
         <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" s="117" t="s">
+      <c r="A10" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B10" s="117" t="s">
+      <c r="B10" s="92" t="s">
         <v>384</v>
       </c>
-      <c r="C10" s="117">
+      <c r="C10" s="92">
         <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" s="117" t="s">
+      <c r="A11" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="92" t="s">
         <v>385</v>
       </c>
-      <c r="C11" s="117">
+      <c r="C11" s="92">
         <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" s="117" t="s">
+      <c r="A12" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="92" t="s">
         <v>386</v>
       </c>
-      <c r="C12" s="117">
+      <c r="C12" s="92">
         <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="117" t="s">
+      <c r="A13" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B13" s="117" t="s">
+      <c r="B13" s="92" t="s">
         <v>387</v>
       </c>
-      <c r="C13" s="117">
+      <c r="C13" s="92">
         <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B14" s="117" t="s">
+      <c r="B14" s="92" t="s">
         <v>388</v>
       </c>
-      <c r="C14" s="117">
+      <c r="C14" s="92">
         <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" s="117" t="s">
+      <c r="A15" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B15" s="117" t="s">
+      <c r="B15" s="92" t="s">
         <v>389</v>
       </c>
-      <c r="C15" s="117">
+      <c r="C15" s="92">
         <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="117" t="s">
+      <c r="A16" s="92" t="s">
         <v>379</v>
       </c>
-      <c r="B16" s="117" t="s">
+      <c r="B16" s="92" t="s">
         <v>390</v>
       </c>
-      <c r="C16" s="117">
+      <c r="C16" s="92">
         <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="117" t="s">
+      <c r="A17" s="92" t="s">
         <v>391</v>
       </c>
-      <c r="B17" s="117" t="s">
+      <c r="B17" s="92" t="s">
         <v>392</v>
       </c>
-      <c r="C17" s="117">
+      <c r="C17" s="92">
         <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="117" t="s">
+      <c r="A18" s="92" t="s">
         <v>391</v>
       </c>
-      <c r="B18" s="117" t="s">
+      <c r="B18" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="117">
+      <c r="C18" s="92">
         <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="117" t="s">
+      <c r="A19" s="92" t="s">
         <v>393</v>
       </c>
-      <c r="B19" s="117" t="s">
+      <c r="B19" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="117">
+      <c r="C19" s="92">
         <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="117" t="s">
+      <c r="A20" s="92" t="s">
         <v>393</v>
       </c>
-      <c r="B20" s="117" t="s">
+      <c r="B20" s="92" t="s">
         <v>394</v>
       </c>
-      <c r="C20" s="117">
+      <c r="C20" s="92">
         <v>119</v>
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="117" t="s">
+      <c r="A21" s="92" t="s">
         <v>393</v>
       </c>
-      <c r="B21" s="117" t="s">
+      <c r="B21" s="92" t="s">
         <v>395</v>
       </c>
-      <c r="C21" s="117">
+      <c r="C21" s="92">
         <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="117" t="s">
+      <c r="A22" s="92" t="s">
         <v>393</v>
       </c>
-      <c r="B22" s="117" t="s">
+      <c r="B22" s="92" t="s">
         <v>396</v>
       </c>
-      <c r="C22" s="117">
+      <c r="C22" s="92">
         <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="117" t="s">
+      <c r="A23" s="92" t="s">
         <v>393</v>
       </c>
-      <c r="B23" s="117" t="s">
+      <c r="B23" s="92" t="s">
         <v>397</v>
       </c>
-      <c r="C23" s="117">
+      <c r="C23" s="92">
         <v>122</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="117" t="s">
+      <c r="A24" s="92" t="s">
         <v>393</v>
       </c>
-      <c r="B24" s="117" t="s">
+      <c r="B24" s="92" t="s">
         <v>398</v>
       </c>
-      <c r="C24" s="117">
+      <c r="C24" s="92">
         <v>123</v>
       </c>
     </row>
@@ -6901,8 +6901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53B4855-AF4D-654D-8FED-46A995940AAB}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6919,32 +6919,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31" customHeight="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="92" t="s">
+      <c r="B1" s="101" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="98" t="s">
+      <c r="D1" s="108" t="s">
         <v>117</v>
       </c>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
       <c r="G1" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="H1" s="96" t="s">
+      <c r="H1" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="I1" s="97"/>
+      <c r="I1" s="110"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="51">
-      <c r="A2" s="91"/>
-      <c r="B2" s="93"/>
-      <c r="C2" s="95"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="104"/>
       <c r="D2" s="23" t="s">
         <v>288</v>
       </c>
@@ -6971,7 +6971,7 @@
       <c r="B3" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="99" t="s">
+      <c r="C3" s="105" t="s">
         <v>39</v>
       </c>
       <c r="D3" s="28">
@@ -6993,10 +6993,10 @@
       <c r="A4" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="112" t="s">
+      <c r="B4" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="100"/>
+      <c r="C4" s="106"/>
       <c r="D4" s="29">
         <v>1</v>
       </c>
@@ -7016,10 +7016,10 @@
       <c r="A5" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="112" t="s">
+      <c r="B5" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="100"/>
+      <c r="C5" s="106"/>
       <c r="D5" s="29">
         <v>1</v>
       </c>
@@ -7039,10 +7039,10 @@
       <c r="A6" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="112" t="s">
+      <c r="B6" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="100"/>
+      <c r="C6" s="106"/>
       <c r="D6" s="29">
         <v>1</v>
       </c>
@@ -7062,10 +7062,10 @@
       <c r="A7" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="112" t="s">
+      <c r="B7" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="100"/>
+      <c r="C7" s="106"/>
       <c r="D7" s="29">
         <v>1</v>
       </c>
@@ -7085,10 +7085,10 @@
       <c r="A8" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="112" t="s">
+      <c r="B8" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="100"/>
+      <c r="C8" s="106"/>
       <c r="D8" s="29">
         <v>1</v>
       </c>
@@ -7108,10 +7108,10 @@
       <c r="A9" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="112" t="s">
+      <c r="B9" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="100"/>
+      <c r="C9" s="106"/>
       <c r="D9" s="29">
         <v>1</v>
       </c>
@@ -7131,10 +7131,10 @@
       <c r="A10" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="87" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="100"/>
+      <c r="C10" s="106"/>
       <c r="D10" s="29">
         <v>1</v>
       </c>
@@ -7154,10 +7154,10 @@
       <c r="A11" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="100"/>
+      <c r="C11" s="106"/>
       <c r="D11" s="29">
         <v>1</v>
       </c>
@@ -7177,10 +7177,10 @@
       <c r="A12" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="100"/>
+      <c r="C12" s="106"/>
       <c r="D12" s="29">
         <v>1</v>
       </c>
@@ -7196,10 +7196,10 @@
       <c r="A13" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="112" t="s">
+      <c r="B13" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="C13" s="100"/>
+      <c r="C13" s="106"/>
       <c r="D13" s="29">
         <v>1</v>
       </c>
@@ -7213,10 +7213,10 @@
       <c r="A14" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="112" t="s">
+      <c r="B14" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="C14" s="100"/>
+      <c r="C14" s="106"/>
       <c r="D14" s="29">
         <v>1</v>
       </c>
@@ -7230,10 +7230,10 @@
       <c r="A15" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="112" t="s">
+      <c r="B15" s="87" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="100"/>
+      <c r="C15" s="106"/>
       <c r="D15" s="29">
         <v>1</v>
       </c>
@@ -7250,7 +7250,7 @@
       <c r="B16" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="C16" s="101"/>
+      <c r="C16" s="107"/>
       <c r="D16" s="30">
         <v>1</v>
       </c>
@@ -7267,7 +7267,7 @@
       <c r="B17" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="99" t="s">
+      <c r="C17" s="105" t="s">
         <v>39</v>
       </c>
       <c r="D17" s="28">
@@ -7289,10 +7289,10 @@
       <c r="A18" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="B18" s="112" t="s">
+      <c r="B18" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="100"/>
+      <c r="C18" s="106"/>
       <c r="D18" s="29">
         <v>1</v>
       </c>
@@ -7312,10 +7312,10 @@
       <c r="A19" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="B19" s="112" t="s">
+      <c r="B19" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="C19" s="100"/>
+      <c r="C19" s="106"/>
       <c r="D19" s="29">
         <v>1</v>
       </c>
@@ -7331,10 +7331,10 @@
       <c r="A20" s="36" t="s">
         <v>111</v>
       </c>
-      <c r="B20" s="112" t="s">
+      <c r="B20" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="100"/>
+      <c r="C20" s="106"/>
       <c r="D20" s="29">
         <v>1</v>
       </c>
@@ -7350,10 +7350,10 @@
       <c r="A21" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="112" t="s">
+      <c r="B21" s="87" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="100" t="s">
+      <c r="C21" s="106" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="29"/>
@@ -7371,10 +7371,10 @@
       <c r="A22" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="112" t="s">
+      <c r="B22" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="100"/>
+      <c r="C22" s="106"/>
       <c r="D22" s="29"/>
       <c r="E22" s="5">
         <v>1</v>
@@ -7390,10 +7390,10 @@
       <c r="A23" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="B23" s="112" t="s">
+      <c r="B23" s="87" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="100"/>
+      <c r="C23" s="106"/>
       <c r="D23" s="29"/>
       <c r="E23" s="5">
         <v>1</v>
@@ -7409,10 +7409,10 @@
       <c r="A24" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="B24" s="112" t="s">
+      <c r="B24" s="87" t="s">
         <v>152</v>
       </c>
-      <c r="C24" s="100"/>
+      <c r="C24" s="106"/>
       <c r="D24" s="29"/>
       <c r="E24" s="5">
         <v>1</v>
@@ -7428,10 +7428,10 @@
       <c r="A25" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B25" s="112" t="s">
+      <c r="B25" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="100"/>
+      <c r="C25" s="106"/>
       <c r="D25" s="29"/>
       <c r="E25" s="5">
         <v>1</v>
@@ -7447,10 +7447,10 @@
       <c r="A26" s="36" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="112" t="s">
+      <c r="B26" s="87" t="s">
         <v>113</v>
       </c>
-      <c r="C26" s="100"/>
+      <c r="C26" s="106"/>
       <c r="D26" s="29"/>
       <c r="E26" s="5">
         <v>1</v>
@@ -7469,7 +7469,7 @@
       <c r="B27" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="101"/>
+      <c r="C27" s="107"/>
       <c r="D27" s="30"/>
       <c r="E27" s="25">
         <v>1</v>
@@ -7483,14 +7483,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="H1:I1"/>
     <mergeCell ref="C3:C16"/>
     <mergeCell ref="C21:C27"/>
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8904,15 +8904,15 @@
       <c r="AD34" s="55"/>
     </row>
     <row r="35" spans="1:30">
-      <c r="A35" s="105" t="s">
+      <c r="A35" s="117" t="s">
         <v>158</v>
       </c>
-      <c r="B35" s="105" t="s">
+      <c r="B35" s="117" t="s">
         <v>249</v>
       </c>
-      <c r="C35" s="105"/>
-      <c r="D35" s="108"/>
-      <c r="E35" s="108"/>
+      <c r="C35" s="117"/>
+      <c r="D35" s="111"/>
+      <c r="E35" s="111"/>
       <c r="F35" s="52"/>
       <c r="G35" s="55"/>
       <c r="H35" s="55"/>
@@ -8940,11 +8940,11 @@
       <c r="AD35" s="55"/>
     </row>
     <row r="36" spans="1:30">
-      <c r="A36" s="106"/>
-      <c r="B36" s="106"/>
-      <c r="C36" s="106"/>
-      <c r="D36" s="109"/>
-      <c r="E36" s="109"/>
+      <c r="A36" s="118"/>
+      <c r="B36" s="118"/>
+      <c r="C36" s="118"/>
+      <c r="D36" s="112"/>
+      <c r="E36" s="112"/>
       <c r="F36" s="52"/>
       <c r="G36" s="55"/>
       <c r="H36" s="55"/>
@@ -8972,11 +8972,11 @@
       <c r="AD36" s="55"/>
     </row>
     <row r="37" spans="1:30">
-      <c r="A37" s="107"/>
-      <c r="B37" s="107"/>
-      <c r="C37" s="107"/>
-      <c r="D37" s="110"/>
-      <c r="E37" s="110"/>
+      <c r="A37" s="119"/>
+      <c r="B37" s="119"/>
+      <c r="C37" s="119"/>
+      <c r="D37" s="113"/>
+      <c r="E37" s="113"/>
       <c r="F37" s="52"/>
       <c r="G37" s="55"/>
       <c r="H37" s="55"/>
@@ -9670,15 +9670,15 @@
       <c r="AD54" s="55"/>
     </row>
     <row r="55" spans="1:30">
-      <c r="A55" s="102" t="s">
+      <c r="A55" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="105" t="s">
+      <c r="B55" s="117" t="s">
         <v>254</v>
       </c>
-      <c r="C55" s="105"/>
-      <c r="D55" s="108"/>
-      <c r="E55" s="108"/>
+      <c r="C55" s="117"/>
+      <c r="D55" s="111"/>
+      <c r="E55" s="111"/>
       <c r="F55" s="65"/>
       <c r="G55" s="55"/>
       <c r="H55" s="55"/>
@@ -9706,11 +9706,11 @@
       <c r="AD55" s="55"/>
     </row>
     <row r="56" spans="1:30">
-      <c r="A56" s="103"/>
-      <c r="B56" s="106"/>
-      <c r="C56" s="106"/>
-      <c r="D56" s="109"/>
-      <c r="E56" s="109"/>
+      <c r="A56" s="115"/>
+      <c r="B56" s="118"/>
+      <c r="C56" s="118"/>
+      <c r="D56" s="112"/>
+      <c r="E56" s="112"/>
       <c r="F56" s="55"/>
       <c r="G56" s="55"/>
       <c r="H56" s="55"/>
@@ -9738,11 +9738,11 @@
       <c r="AD56" s="55"/>
     </row>
     <row r="57" spans="1:30">
-      <c r="A57" s="103"/>
-      <c r="B57" s="106"/>
-      <c r="C57" s="106"/>
-      <c r="D57" s="109"/>
-      <c r="E57" s="109"/>
+      <c r="A57" s="115"/>
+      <c r="B57" s="118"/>
+      <c r="C57" s="118"/>
+      <c r="D57" s="112"/>
+      <c r="E57" s="112"/>
       <c r="F57" s="65"/>
       <c r="G57" s="55"/>
       <c r="H57" s="55"/>
@@ -9770,11 +9770,11 @@
       <c r="AD57" s="55"/>
     </row>
     <row r="58" spans="1:30">
-      <c r="A58" s="104"/>
-      <c r="B58" s="107"/>
-      <c r="C58" s="107"/>
-      <c r="D58" s="110"/>
-      <c r="E58" s="110"/>
+      <c r="A58" s="116"/>
+      <c r="B58" s="119"/>
+      <c r="C58" s="119"/>
+      <c r="D58" s="113"/>
+      <c r="E58" s="113"/>
       <c r="F58" s="65"/>
       <c r="G58" s="55"/>
       <c r="H58" s="55"/>
@@ -10042,15 +10042,15 @@
       <c r="AD64" s="55"/>
     </row>
     <row r="65" spans="1:30" s="6" customFormat="1">
-      <c r="A65" s="102" t="s">
+      <c r="A65" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="105" t="s">
+      <c r="B65" s="117" t="s">
         <v>258</v>
       </c>
-      <c r="C65" s="105"/>
-      <c r="D65" s="108"/>
-      <c r="E65" s="108"/>
+      <c r="C65" s="117"/>
+      <c r="D65" s="111"/>
+      <c r="E65" s="111"/>
       <c r="F65" s="65"/>
       <c r="G65" s="55"/>
       <c r="H65" s="55"/>
@@ -10078,11 +10078,11 @@
       <c r="AD65" s="55"/>
     </row>
     <row r="66" spans="1:30" s="6" customFormat="1">
-      <c r="A66" s="103"/>
-      <c r="B66" s="106"/>
-      <c r="C66" s="106"/>
-      <c r="D66" s="109"/>
-      <c r="E66" s="109"/>
+      <c r="A66" s="115"/>
+      <c r="B66" s="118"/>
+      <c r="C66" s="118"/>
+      <c r="D66" s="112"/>
+      <c r="E66" s="112"/>
       <c r="F66" s="65"/>
       <c r="G66" s="55"/>
       <c r="H66" s="55"/>
@@ -10110,11 +10110,11 @@
       <c r="AD66" s="55"/>
     </row>
     <row r="67" spans="1:30">
-      <c r="A67" s="104"/>
-      <c r="B67" s="107"/>
-      <c r="C67" s="107"/>
-      <c r="D67" s="110"/>
-      <c r="E67" s="110"/>
+      <c r="A67" s="116"/>
+      <c r="B67" s="119"/>
+      <c r="C67" s="119"/>
+      <c r="D67" s="113"/>
+      <c r="E67" s="113"/>
       <c r="F67" s="65"/>
       <c r="G67" s="55"/>
       <c r="H67" s="55"/>
@@ -10211,12 +10211,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
     <mergeCell ref="A65:A67"/>
     <mergeCell ref="B65:B67"/>
     <mergeCell ref="C65:C67"/>
@@ -10226,6 +10220,12 @@
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="B55:B58"/>
     <mergeCell ref="C35:C37"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="D55:D58"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10356,7 +10356,7 @@
       </c>
     </row>
     <row r="2" spans="1:27" ht="17">
-      <c r="A2" s="111" t="s">
+      <c r="A2" s="120" t="s">
         <v>82</v>
       </c>
       <c r="B2" s="81" t="s">
@@ -10464,7 +10464,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" ht="17">
-      <c r="A3" s="111"/>
+      <c r="A3" s="120"/>
       <c r="B3" s="81" t="s">
         <v>61</v>
       </c>
@@ -10546,7 +10546,7 @@
       </c>
     </row>
     <row r="4" spans="1:27" ht="17">
-      <c r="A4" s="111" t="s">
+      <c r="A4" s="120" t="s">
         <v>83</v>
       </c>
       <c r="B4" s="81" t="s">
@@ -10654,7 +10654,7 @@
       </c>
     </row>
     <row r="5" spans="1:27" ht="17">
-      <c r="A5" s="111"/>
+      <c r="A5" s="120"/>
       <c r="B5" s="81" t="s">
         <v>61</v>
       </c>
@@ -10736,7 +10736,7 @@
       </c>
     </row>
     <row r="6" spans="1:27" ht="17">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="120" t="s">
         <v>86</v>
       </c>
       <c r="B6" s="81" t="s">
@@ -10844,7 +10844,7 @@
       </c>
     </row>
     <row r="7" spans="1:27" ht="17">
-      <c r="A7" s="111"/>
+      <c r="A7" s="120"/>
       <c r="B7" s="81" t="s">
         <v>61</v>
       </c>
@@ -15317,7 +15317,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
fix: modify python code
</commit_message>
<xml_diff>
--- a/成本核算数据源配置表.xlsx
+++ b/成本核算数据源配置表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinliao/Projects/gitclone/python-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6F592C-8CF3-C342-B517-0AD6606EBBE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A497D7D8-B0E9-BD4E-BECE-37D9A28A6C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68940" yWindow="-820" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{97E2786A-046E-A540-BAE7-43526A264538}"/>
+    <workbookView xWindow="-68960" yWindow="-840" windowWidth="28800" windowHeight="17500" xr2:uid="{97E2786A-046E-A540-BAE7-43526A264538}"/>
   </bookViews>
   <sheets>
     <sheet name="人员费用配置表" sheetId="20" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="405">
   <si>
     <t>人员</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -570,10 +570,6 @@
   </si>
   <si>
     <t>成都天天阿里云服务费</t>
-  </si>
-  <si>
-    <t>成都天天阿里云服务费</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>成都天天Google和AWS云服务费</t>
@@ -1065,9 +1061,6 @@
     <t>schema: 单列，多列</t>
   </si>
   <si>
-    <t>北京天天阿里云服务费</t>
-  </si>
-  <si>
     <t>T1部门分摊费用</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1573,6 +1566,22 @@
   <si>
     <t>研发人员福利费用
 （排除公摊项目）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京天天云服务费用BT</t>
+  </si>
+  <si>
+    <t>成都天天云服务费用CT</t>
+  </si>
+  <si>
+    <t>大乐至简云服务费DL</t>
+  </si>
+  <si>
+    <t>北京运营费用</t>
+  </si>
+  <si>
+    <t>研发中台部</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2197,13 +2206,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2218,10 +2224,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2242,15 +2251,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2268,6 +2268,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2594,8 +2603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC9293E-C443-5D4F-807A-3A2F963837CD}">
   <dimension ref="A1:BO42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -2638,289 +2647,289 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="49" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="101" t="s">
+      <c r="C1" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="101" t="s">
+      <c r="D1" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="101" t="s">
+      <c r="E1" s="100" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="103" t="s">
+      <c r="F1" s="96" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="96" t="s">
+      <c r="G1" s="102" t="s">
+        <v>291</v>
+      </c>
+      <c r="H1" s="103"/>
+      <c r="I1" s="103"/>
+      <c r="J1" s="103"/>
+      <c r="K1" s="103"/>
+      <c r="L1" s="103"/>
+      <c r="M1" s="104"/>
+      <c r="N1" s="102" t="s">
+        <v>292</v>
+      </c>
+      <c r="O1" s="103"/>
+      <c r="P1" s="103"/>
+      <c r="Q1" s="103"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="103"/>
+      <c r="T1" s="104"/>
+      <c r="U1" s="103" t="s">
+        <v>397</v>
+      </c>
+      <c r="V1" s="103"/>
+      <c r="W1" s="103"/>
+      <c r="X1" s="103"/>
+      <c r="Y1" s="103"/>
+      <c r="Z1" s="103"/>
+      <c r="AA1" s="103"/>
+      <c r="AB1" s="103"/>
+      <c r="AC1" s="103"/>
+      <c r="AD1" s="103"/>
+      <c r="AE1" s="103"/>
+      <c r="AF1" s="103"/>
+      <c r="AG1" s="103"/>
+      <c r="AH1" s="103"/>
+      <c r="AI1" s="103"/>
+      <c r="AJ1" s="103"/>
+      <c r="AK1" s="103"/>
+      <c r="AL1" s="102" t="s">
+        <v>398</v>
+      </c>
+      <c r="AM1" s="103"/>
+      <c r="AN1" s="103"/>
+      <c r="AO1" s="103"/>
+      <c r="AP1" s="103"/>
+      <c r="AQ1" s="103"/>
+      <c r="AR1" s="104"/>
+      <c r="AS1" s="102" t="s">
         <v>293</v>
       </c>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="96" t="s">
+      <c r="AT1" s="103"/>
+      <c r="AU1" s="103"/>
+      <c r="AV1" s="103"/>
+      <c r="AW1" s="103"/>
+      <c r="AX1" s="103"/>
+      <c r="AY1" s="103"/>
+      <c r="AZ1" s="104"/>
+      <c r="BA1" s="103" t="s">
         <v>294</v>
       </c>
-      <c r="O1" s="97"/>
-      <c r="P1" s="97"/>
-      <c r="Q1" s="97"/>
-      <c r="R1" s="97"/>
-      <c r="S1" s="97"/>
-      <c r="T1" s="98"/>
-      <c r="U1" s="97" t="s">
+      <c r="BB1" s="103"/>
+      <c r="BC1" s="104"/>
+      <c r="BD1" s="102" t="s">
+        <v>295</v>
+      </c>
+      <c r="BE1" s="103"/>
+      <c r="BF1" s="103"/>
+      <c r="BG1" s="103"/>
+      <c r="BH1" s="103"/>
+      <c r="BI1" s="103"/>
+      <c r="BJ1" s="103"/>
+      <c r="BK1" s="103"/>
+      <c r="BL1" s="103"/>
+      <c r="BM1" s="103"/>
+      <c r="BN1" s="103"/>
+      <c r="BO1" s="104"/>
+    </row>
+    <row r="2" spans="1:67" s="1" customFormat="1" ht="68">
+      <c r="A2" s="99"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="97"/>
+      <c r="G2" s="22" t="s">
+        <v>296</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>303</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="U2" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="AL2" s="26" t="s">
         <v>399</v>
       </c>
-      <c r="V1" s="97"/>
-      <c r="W1" s="97"/>
-      <c r="X1" s="97"/>
-      <c r="Y1" s="97"/>
-      <c r="Z1" s="97"/>
-      <c r="AA1" s="97"/>
-      <c r="AB1" s="97"/>
-      <c r="AC1" s="97"/>
-      <c r="AD1" s="97"/>
-      <c r="AE1" s="97"/>
-      <c r="AF1" s="97"/>
-      <c r="AG1" s="97"/>
-      <c r="AH1" s="97"/>
-      <c r="AI1" s="97"/>
-      <c r="AJ1" s="97"/>
-      <c r="AK1" s="97"/>
-      <c r="AL1" s="96" t="s">
-        <v>400</v>
-      </c>
-      <c r="AM1" s="97"/>
-      <c r="AN1" s="97"/>
-      <c r="AO1" s="97"/>
-      <c r="AP1" s="97"/>
-      <c r="AQ1" s="97"/>
-      <c r="AR1" s="98"/>
-      <c r="AS1" s="96" t="s">
-        <v>295</v>
-      </c>
-      <c r="AT1" s="97"/>
-      <c r="AU1" s="97"/>
-      <c r="AV1" s="97"/>
-      <c r="AW1" s="97"/>
-      <c r="AX1" s="97"/>
-      <c r="AY1" s="97"/>
-      <c r="AZ1" s="98"/>
-      <c r="BA1" s="97" t="s">
-        <v>296</v>
-      </c>
-      <c r="BB1" s="97"/>
-      <c r="BC1" s="98"/>
-      <c r="BD1" s="96" t="s">
+      <c r="AM2" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="BE1" s="97"/>
-      <c r="BF1" s="97"/>
-      <c r="BG1" s="97"/>
-      <c r="BH1" s="97"/>
-      <c r="BI1" s="97"/>
-      <c r="BJ1" s="97"/>
-      <c r="BK1" s="97"/>
-      <c r="BL1" s="97"/>
-      <c r="BM1" s="97"/>
-      <c r="BN1" s="97"/>
-      <c r="BO1" s="98"/>
-    </row>
-    <row r="2" spans="1:67" s="1" customFormat="1" ht="68">
-      <c r="A2" s="100"/>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="22" t="s">
+      <c r="AN2" s="4" t="s">
         <v>298</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="AO2" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>305</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="U2" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AS2" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="AF2" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="AH2" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="AK2" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="AL2" s="26" t="s">
-        <v>401</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="AN2" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="AO2" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="AP2" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="AQ2" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="AR2" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="AS2" s="22" t="s">
+      <c r="AU2" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
         <v>313</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AY2" s="4" t="s">
         <v>314</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AZ2" s="4" t="s">
         <v>315</v>
       </c>
-      <c r="AY2" s="4" t="s">
+      <c r="BA2" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BB2" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="BA2" s="26" t="s">
+      <c r="BC2" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="BB2" s="4" t="s">
+      <c r="BD2" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="BC2" s="15" t="s">
+      <c r="BE2" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="BD2" s="22" t="s">
+      <c r="BF2" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="BE2" s="22" t="s">
+      <c r="BG2" s="22" t="s">
         <v>322</v>
       </c>
-      <c r="BF2" s="22" t="s">
+      <c r="BH2" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="BG2" s="22" t="s">
+      <c r="BI2" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="BH2" s="22" t="s">
+      <c r="BJ2" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="BI2" s="4" t="s">
+      <c r="BK2" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BL2" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="BK2" s="4" t="s">
+      <c r="BM2" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="BL2" s="4" t="s">
+      <c r="BN2" s="4" t="s">
         <v>329</v>
       </c>
-      <c r="BM2" s="4" t="s">
+      <c r="BO2" s="15" t="s">
         <v>330</v>
-      </c>
-      <c r="BN2" s="4" t="s">
-        <v>331</v>
-      </c>
-      <c r="BO2" s="15" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:67" s="1" customFormat="1" ht="85">
@@ -2943,187 +2952,187 @@
         <v>120</v>
       </c>
       <c r="G3" s="23" t="s">
+        <v>331</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="L3" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="M3" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="L3" s="14" t="s">
+      <c r="N3" s="23" t="s">
         <v>338</v>
       </c>
-      <c r="M3" s="14" t="s">
+      <c r="O3" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="U3" s="23" t="s">
         <v>339</v>
       </c>
-      <c r="N3" s="23" t="s">
+      <c r="V3" s="23" t="s">
+        <v>230</v>
+      </c>
+      <c r="W3" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="O3" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="Q3" s="14" t="s">
+      <c r="X3" s="23" t="s">
+        <v>341</v>
+      </c>
+      <c r="Y3" s="23" t="s">
+        <v>342</v>
+      </c>
+      <c r="Z3" s="23" t="s">
+        <v>343</v>
+      </c>
+      <c r="AA3" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="AB3" s="23" t="s">
+        <v>344</v>
+      </c>
+      <c r="AC3" s="23" t="s">
+        <v>345</v>
+      </c>
+      <c r="AD3" s="23" t="s">
+        <v>346</v>
+      </c>
+      <c r="AE3" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="AF3" s="14" t="s">
+        <v>348</v>
+      </c>
+      <c r="AG3" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="AH3" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="AI3" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="AJ3" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="AK3" s="14" t="s">
         <v>337</v>
       </c>
-      <c r="S3" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="T3" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="U3" s="23" t="s">
-        <v>341</v>
-      </c>
-      <c r="V3" s="23" t="s">
-        <v>231</v>
-      </c>
-      <c r="W3" s="23" t="s">
-        <v>342</v>
-      </c>
-      <c r="X3" s="23" t="s">
-        <v>343</v>
-      </c>
-      <c r="Y3" s="23" t="s">
-        <v>344</v>
-      </c>
-      <c r="Z3" s="23" t="s">
-        <v>345</v>
-      </c>
-      <c r="AA3" s="23" t="s">
-        <v>232</v>
-      </c>
-      <c r="AB3" s="23" t="s">
-        <v>346</v>
-      </c>
-      <c r="AC3" s="23" t="s">
+      <c r="AL3" s="23" t="s">
         <v>347</v>
       </c>
-      <c r="AD3" s="23" t="s">
+      <c r="AM3" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="AE3" s="14" t="s">
+      <c r="AN3" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="AO3" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="AF3" s="14" t="s">
+      <c r="AP3" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="AG3" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="AH3" s="14" t="s">
+      <c r="AQ3" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="AR3" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="AS3" s="23" t="s">
         <v>351</v>
       </c>
-      <c r="AI3" s="14" t="s">
+      <c r="AT3" s="23" t="s">
         <v>352</v>
       </c>
-      <c r="AJ3" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="AK3" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="AL3" s="23" t="s">
-        <v>349</v>
-      </c>
-      <c r="AM3" s="14" t="s">
-        <v>350</v>
-      </c>
-      <c r="AN3" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="AO3" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="AP3" s="14" t="s">
-        <v>352</v>
-      </c>
-      <c r="AQ3" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="AR3" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="AS3" s="23" t="s">
+      <c r="AU3" s="23" t="s">
         <v>353</v>
       </c>
-      <c r="AT3" s="23" t="s">
+      <c r="AV3" s="14" t="s">
         <v>354</v>
       </c>
-      <c r="AU3" s="23" t="s">
+      <c r="AW3" s="14" t="s">
         <v>355</v>
       </c>
-      <c r="AV3" s="14" t="s">
+      <c r="AX3" s="14" t="s">
         <v>356</v>
       </c>
-      <c r="AW3" s="14" t="s">
+      <c r="AY3" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="AX3" s="14" t="s">
+      <c r="AZ3" s="14" t="s">
         <v>358</v>
       </c>
-      <c r="AY3" s="14" t="s">
+      <c r="BA3" s="88" t="s">
         <v>359</v>
       </c>
-      <c r="AZ3" s="14" t="s">
+      <c r="BB3" s="89" t="s">
         <v>360</v>
       </c>
-      <c r="BA3" s="88" t="s">
+      <c r="BC3" s="90" t="s">
         <v>361</v>
       </c>
-      <c r="BB3" s="89" t="s">
+      <c r="BD3" s="23" t="s">
         <v>362</v>
       </c>
-      <c r="BC3" s="90" t="s">
+      <c r="BE3" s="14" t="s">
         <v>363</v>
       </c>
-      <c r="BD3" s="23" t="s">
+      <c r="BF3" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="BE3" s="14" t="s">
+      <c r="BG3" s="14" t="s">
         <v>365</v>
       </c>
-      <c r="BF3" s="14" t="s">
+      <c r="BH3" s="14" t="s">
         <v>366</v>
       </c>
-      <c r="BG3" s="14" t="s">
+      <c r="BI3" s="14" t="s">
         <v>367</v>
       </c>
-      <c r="BH3" s="14" t="s">
+      <c r="BJ3" s="14" t="s">
         <v>368</v>
       </c>
-      <c r="BI3" s="14" t="s">
+      <c r="BK3" s="14" t="s">
         <v>369</v>
       </c>
-      <c r="BJ3" s="14" t="s">
+      <c r="BL3" s="14" t="s">
         <v>370</v>
       </c>
-      <c r="BK3" s="14" t="s">
+      <c r="BM3" s="14" t="s">
         <v>371</v>
       </c>
-      <c r="BL3" s="14" t="s">
+      <c r="BN3" s="14" t="s">
         <v>372</v>
       </c>
-      <c r="BM3" s="14" t="s">
+      <c r="BO3" s="16" t="s">
         <v>373</v>
-      </c>
-      <c r="BN3" s="14" t="s">
-        <v>374</v>
-      </c>
-      <c r="BO3" s="16" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:67" ht="17">
@@ -3145,9 +3154,7 @@
       <c r="F4" s="15">
         <v>1</v>
       </c>
-      <c r="G4" s="22">
-        <v>1</v>
-      </c>
+      <c r="G4" s="22"/>
       <c r="H4" s="4">
         <v>1</v>
       </c>
@@ -3156,9 +3163,7 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="15"/>
-      <c r="N4" s="22">
-        <v>1</v>
-      </c>
+      <c r="N4" s="22"/>
       <c r="O4" s="4">
         <v>1</v>
       </c>
@@ -3188,9 +3193,7 @@
       <c r="AI4" s="4"/>
       <c r="AJ4" s="4"/>
       <c r="AK4" s="4"/>
-      <c r="AL4" s="22">
-        <v>1</v>
-      </c>
+      <c r="AL4" s="22"/>
       <c r="AM4" s="4">
         <v>1</v>
       </c>
@@ -3347,9 +3350,7 @@
       <c r="F6" s="15">
         <v>1</v>
       </c>
-      <c r="G6" s="22">
-        <v>1</v>
-      </c>
+      <c r="G6" s="22"/>
       <c r="H6" s="4">
         <v>1</v>
       </c>
@@ -3358,9 +3359,7 @@
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
       <c r="M6" s="15"/>
-      <c r="N6" s="22">
-        <v>1</v>
-      </c>
+      <c r="N6" s="22"/>
       <c r="O6" s="4">
         <v>1</v>
       </c>
@@ -3390,9 +3389,7 @@
       <c r="AI6" s="4"/>
       <c r="AJ6" s="4"/>
       <c r="AK6" s="4"/>
-      <c r="AL6" s="22">
-        <v>1</v>
-      </c>
+      <c r="AL6" s="22"/>
       <c r="AM6" s="4">
         <v>1</v>
       </c>
@@ -3549,9 +3546,7 @@
       <c r="F8" s="15">
         <v>1</v>
       </c>
-      <c r="G8" s="22">
-        <v>1</v>
-      </c>
+      <c r="G8" s="22"/>
       <c r="H8" s="4">
         <v>1</v>
       </c>
@@ -3560,9 +3555,7 @@
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
       <c r="M8" s="15"/>
-      <c r="N8" s="22">
-        <v>1</v>
-      </c>
+      <c r="N8" s="22"/>
       <c r="O8" s="4">
         <v>1</v>
       </c>
@@ -3592,9 +3585,7 @@
       <c r="AI8" s="4"/>
       <c r="AJ8" s="4"/>
       <c r="AK8" s="4"/>
-      <c r="AL8" s="22">
-        <v>1</v>
-      </c>
+      <c r="AL8" s="22"/>
       <c r="AM8" s="4">
         <v>1</v>
       </c>
@@ -3641,7 +3632,7 @@
         <v>52</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F9" s="15"/>
       <c r="G9" s="22">
@@ -3747,9 +3738,7 @@
       <c r="F10" s="15">
         <v>1</v>
       </c>
-      <c r="G10" s="22">
-        <v>1</v>
-      </c>
+      <c r="G10" s="22"/>
       <c r="H10" s="4">
         <v>1</v>
       </c>
@@ -3758,9 +3747,7 @@
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="15"/>
-      <c r="N10" s="22">
-        <v>1</v>
-      </c>
+      <c r="N10" s="22"/>
       <c r="O10" s="4">
         <v>1</v>
       </c>
@@ -3790,9 +3777,7 @@
       <c r="AI10" s="4"/>
       <c r="AJ10" s="4"/>
       <c r="AK10" s="15"/>
-      <c r="AL10" s="22">
-        <v>1</v>
-      </c>
+      <c r="AL10" s="22"/>
       <c r="AM10" s="4">
         <v>1</v>
       </c>
@@ -3925,9 +3910,7 @@
       <c r="F12" s="15">
         <v>1</v>
       </c>
-      <c r="G12" s="22">
-        <v>1</v>
-      </c>
+      <c r="G12" s="22"/>
       <c r="H12" s="4">
         <v>1</v>
       </c>
@@ -3936,9 +3919,7 @@
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
       <c r="M12" s="15"/>
-      <c r="N12" s="22">
-        <v>1</v>
-      </c>
+      <c r="N12" s="22"/>
       <c r="O12" s="4">
         <v>1</v>
       </c>
@@ -3968,9 +3949,7 @@
       <c r="AI12" s="4"/>
       <c r="AJ12" s="4"/>
       <c r="AK12" s="15"/>
-      <c r="AL12" s="22">
-        <v>1</v>
-      </c>
+      <c r="AL12" s="22"/>
       <c r="AM12" s="4">
         <v>1</v>
       </c>
@@ -4107,9 +4086,7 @@
       <c r="F14" s="17">
         <v>1</v>
       </c>
-      <c r="G14" s="26">
-        <v>1</v>
-      </c>
+      <c r="G14" s="26"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
       <c r="J14" s="11"/>
@@ -4118,9 +4095,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="17"/>
-      <c r="N14" s="26">
-        <v>1</v>
-      </c>
+      <c r="N14" s="26"/>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
@@ -4150,9 +4125,7 @@
         <v>1</v>
       </c>
       <c r="AK14" s="17"/>
-      <c r="AL14" s="26">
-        <v>1</v>
-      </c>
+      <c r="AL14" s="26"/>
       <c r="AM14" s="11"/>
       <c r="AN14" s="11"/>
       <c r="AO14" s="11"/>
@@ -4272,9 +4245,7 @@
       <c r="BB15" s="3">
         <v>1</v>
       </c>
-      <c r="BC15" s="15">
-        <v>1</v>
-      </c>
+      <c r="BC15" s="15"/>
       <c r="BD15" s="22"/>
       <c r="BE15" s="4"/>
       <c r="BF15" s="4"/>
@@ -4311,9 +4282,7 @@
       <c r="F16" s="15">
         <v>1</v>
       </c>
-      <c r="G16" s="22">
-        <v>1</v>
-      </c>
+      <c r="G16" s="22"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
@@ -4322,9 +4291,7 @@
         <v>1</v>
       </c>
       <c r="M16" s="15"/>
-      <c r="N16" s="22">
-        <v>1</v>
-      </c>
+      <c r="N16" s="22"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
@@ -4354,9 +4321,7 @@
         <v>1</v>
       </c>
       <c r="AK16" s="15"/>
-      <c r="AL16" s="22">
-        <v>1</v>
-      </c>
+      <c r="AL16" s="22"/>
       <c r="AM16" s="4"/>
       <c r="AN16" s="4"/>
       <c r="AO16" s="4"/>
@@ -4402,7 +4367,7 @@
         <v>138</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="22">
@@ -4475,9 +4440,7 @@
       <c r="BB17" s="3">
         <v>1</v>
       </c>
-      <c r="BC17" s="15">
-        <v>1</v>
-      </c>
+      <c r="BC17" s="15"/>
       <c r="BD17" s="22"/>
       <c r="BE17" s="4"/>
       <c r="BF17" s="4"/>
@@ -4514,9 +4477,7 @@
       <c r="F18" s="17">
         <v>1</v>
       </c>
-      <c r="G18" s="26">
-        <v>1</v>
-      </c>
+      <c r="G18" s="26"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
       <c r="J18" s="11">
@@ -4525,9 +4486,7 @@
       <c r="K18" s="11"/>
       <c r="L18" s="11"/>
       <c r="M18" s="17"/>
-      <c r="N18" s="26">
-        <v>1</v>
-      </c>
+      <c r="N18" s="26"/>
       <c r="O18" s="11"/>
       <c r="P18" s="11"/>
       <c r="Q18" s="11">
@@ -4557,9 +4516,7 @@
       <c r="AI18" s="11"/>
       <c r="AJ18" s="11"/>
       <c r="AK18" s="17"/>
-      <c r="AL18" s="26">
-        <v>1</v>
-      </c>
+      <c r="AL18" s="26"/>
       <c r="AM18" s="11"/>
       <c r="AN18" s="11"/>
       <c r="AO18" s="11">
@@ -4677,7 +4634,9 @@
         <v>1</v>
       </c>
       <c r="BB19" s="95"/>
-      <c r="BC19" s="15"/>
+      <c r="BC19" s="15">
+        <v>1</v>
+      </c>
       <c r="BD19" s="22"/>
       <c r="BE19" s="4"/>
       <c r="BF19" s="4"/>
@@ -4712,9 +4671,7 @@
       <c r="F20" s="15">
         <v>1</v>
       </c>
-      <c r="G20" s="22">
-        <v>1</v>
-      </c>
+      <c r="G20" s="22"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4">
@@ -4723,9 +4680,7 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
       <c r="M20" s="15"/>
-      <c r="N20" s="22">
-        <v>1</v>
-      </c>
+      <c r="N20" s="22"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="4">
@@ -4755,9 +4710,7 @@
       <c r="AI20" s="4"/>
       <c r="AJ20" s="4"/>
       <c r="AK20" s="15"/>
-      <c r="AL20" s="22">
-        <v>1</v>
-      </c>
+      <c r="AL20" s="22"/>
       <c r="AM20" s="4"/>
       <c r="AN20" s="4"/>
       <c r="AO20" s="4">
@@ -4804,7 +4757,7 @@
         <v>53</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F21" s="15"/>
       <c r="G21" s="22">
@@ -4875,7 +4828,9 @@
         <v>1</v>
       </c>
       <c r="BB21" s="95"/>
-      <c r="BC21" s="15"/>
+      <c r="BC21" s="15">
+        <v>1</v>
+      </c>
       <c r="BD21" s="22"/>
       <c r="BE21" s="4"/>
       <c r="BF21" s="4"/>
@@ -4906,9 +4861,7 @@
       <c r="F22" s="15">
         <v>1</v>
       </c>
-      <c r="G22" s="22">
-        <v>1</v>
-      </c>
+      <c r="G22" s="22"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4">
@@ -4917,9 +4870,7 @@
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="15"/>
-      <c r="N22" s="22">
-        <v>1</v>
-      </c>
+      <c r="N22" s="22"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
       <c r="Q22" s="4">
@@ -4949,9 +4900,7 @@
       <c r="AI22" s="4"/>
       <c r="AJ22" s="4"/>
       <c r="AK22" s="15"/>
-      <c r="AL22" s="22">
-        <v>1</v>
-      </c>
+      <c r="AL22" s="22"/>
       <c r="AM22" s="4"/>
       <c r="AN22" s="4"/>
       <c r="AO22" s="4">
@@ -5071,13 +5020,13 @@
     </row>
     <row r="24" spans="1:67" ht="34">
       <c r="A24" s="26" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="11"/>
@@ -5152,13 +5101,13 @@
     </row>
     <row r="25" spans="1:67" ht="34">
       <c r="A25" s="22" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -5233,13 +5182,13 @@
     </row>
     <row r="26" spans="1:67" ht="34">
       <c r="A26" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -5313,13 +5262,13 @@
     </row>
     <row r="27" spans="1:67" ht="34">
       <c r="A27" s="22" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -5394,7 +5343,7 @@
     </row>
     <row r="28" spans="1:67" ht="17">
       <c r="A28" s="26" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>40</v>
@@ -5475,7 +5424,7 @@
     </row>
     <row r="29" spans="1:67" ht="17">
       <c r="A29" s="22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>40</v>
@@ -5558,7 +5507,7 @@
     </row>
     <row r="30" spans="1:67" ht="17">
       <c r="A30" s="24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B30" s="13" t="s">
         <v>40</v>
@@ -6598,12 +6547,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="BD1:BO1"/>
     <mergeCell ref="G1:M1"/>
     <mergeCell ref="N1:T1"/>
@@ -6611,6 +6554,12 @@
     <mergeCell ref="AL1:AR1"/>
     <mergeCell ref="AS1:AZ1"/>
     <mergeCell ref="BA1:BC1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6619,28 +6568,28 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E4309A5-7274-AE4A-AEE5-4D23B26A45EE}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:3" ht="17">
       <c r="A1" s="91" t="s">
+        <v>374</v>
+      </c>
+      <c r="B1" s="91" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1" s="91" t="s">
         <v>376</v>
-      </c>
-      <c r="B1" s="91" t="s">
-        <v>377</v>
-      </c>
-      <c r="C1" s="91" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B2" s="92" t="s">
         <v>67</v>
@@ -6651,7 +6600,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B3" s="92" t="s">
         <v>65</v>
@@ -6662,7 +6611,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B4" s="92" t="s">
         <v>66</v>
@@ -6673,7 +6622,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B5" s="92" t="s">
         <v>68</v>
@@ -6684,10 +6633,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B6" s="92" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C6" s="92">
         <v>105</v>
@@ -6695,10 +6644,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="92" t="s">
+        <v>377</v>
+      </c>
+      <c r="B7" s="92" t="s">
         <v>379</v>
-      </c>
-      <c r="B7" s="92" t="s">
-        <v>381</v>
       </c>
       <c r="C7" s="92">
         <v>106</v>
@@ -6706,10 +6655,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B8" s="92" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C8" s="92">
         <v>107</v>
@@ -6717,10 +6666,10 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B9" s="92" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C9" s="92">
         <v>108</v>
@@ -6728,10 +6677,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B10" s="92" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C10" s="92">
         <v>109</v>
@@ -6739,10 +6688,10 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C11" s="92">
         <v>110</v>
@@ -6750,10 +6699,10 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B12" s="92" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C12" s="92">
         <v>111</v>
@@ -6761,10 +6710,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B13" s="92" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C13" s="92">
         <v>112</v>
@@ -6772,10 +6721,10 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C14" s="92">
         <v>113</v>
@@ -6783,10 +6732,10 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="C15" s="92">
         <v>114</v>
@@ -6794,10 +6743,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="92" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B16" s="92" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C16" s="92">
         <v>115</v>
@@ -6805,10 +6754,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="92" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B17" s="92" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="C17" s="92">
         <v>116</v>
@@ -6816,7 +6765,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="92" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B18" s="92" t="s">
         <v>66</v>
@@ -6827,7 +6776,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="92" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B19" s="92" t="s">
         <v>66</v>
@@ -6838,10 +6787,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="92" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B20" s="92" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C20" s="92">
         <v>119</v>
@@ -6849,10 +6798,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="92" t="s">
+        <v>391</v>
+      </c>
+      <c r="B21" s="92" t="s">
         <v>393</v>
-      </c>
-      <c r="B21" s="92" t="s">
-        <v>395</v>
       </c>
       <c r="C21" s="92">
         <v>120</v>
@@ -6860,10 +6809,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="92" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B22" s="92" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C22" s="92">
         <v>121</v>
@@ -6871,10 +6820,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="92" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B23" s="92" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C23" s="92">
         <v>122</v>
@@ -6882,13 +6831,24 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="92" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B24" s="92" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C24" s="92">
         <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="92" t="s">
+        <v>391</v>
+      </c>
+      <c r="B25" s="92" t="s">
+        <v>404</v>
+      </c>
+      <c r="C25" s="92">
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -6901,8 +6861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53B4855-AF4D-654D-8FED-46A995940AAB}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6919,13 +6879,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="31" customHeight="1">
-      <c r="A1" s="99" t="s">
+      <c r="A1" s="98" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="101" t="s">
+      <c r="B1" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="103" t="s">
+      <c r="C1" s="96" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="108" t="s">
@@ -6937,31 +6897,31 @@
         <v>118</v>
       </c>
       <c r="H1" s="109" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I1" s="110"/>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="51">
-      <c r="A2" s="100"/>
-      <c r="B2" s="102"/>
-      <c r="C2" s="104"/>
+      <c r="A2" s="99"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="97"/>
       <c r="D2" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="G2" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="H2" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="I2" s="16" t="s">
         <v>290</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>228</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -7410,7 +7370,7 @@
         <v>104</v>
       </c>
       <c r="B24" s="87" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C24" s="106"/>
       <c r="D24" s="29"/>
@@ -7540,10 +7500,10 @@
         <v>16</v>
       </c>
       <c r="D1" s="43" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E1" s="43" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F1" s="44" t="s">
         <v>87</v>
@@ -7626,7 +7586,7 @@
         <v>17</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C2" s="45"/>
       <c r="D2" s="46"/>
@@ -7662,10 +7622,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="54" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="48"/>
@@ -7700,10 +7660,10 @@
         <v>19</v>
       </c>
       <c r="B4" s="54" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="49" t="s">
         <v>175</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>176</v>
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="48"/>
@@ -7772,16 +7732,16 @@
         <v>115</v>
       </c>
       <c r="B6" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="C6" s="50" t="s">
-        <v>178</v>
-      </c>
       <c r="D6" s="51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E6" s="71" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F6" s="52"/>
       <c r="G6" s="55"/>
@@ -7814,13 +7774,13 @@
         <v>116</v>
       </c>
       <c r="B7" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="C7" s="50" t="s">
-        <v>178</v>
-      </c>
       <c r="D7" s="51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E7" s="72"/>
       <c r="F7" s="52"/>
@@ -7854,13 +7814,13 @@
         <v>149</v>
       </c>
       <c r="B8" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="50" t="s">
-        <v>178</v>
-      </c>
       <c r="D8" s="51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E8" s="51"/>
       <c r="F8" s="52"/>
@@ -7891,16 +7851,16 @@
     </row>
     <row r="9" spans="1:30" ht="38">
       <c r="A9" s="70" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="50" t="s">
-        <v>178</v>
-      </c>
       <c r="D9" s="51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E9" s="51"/>
       <c r="F9" s="52"/>
@@ -7931,16 +7891,16 @@
     </row>
     <row r="10" spans="1:30" ht="19">
       <c r="A10" s="70" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="50" t="s">
         <v>177</v>
       </c>
-      <c r="C10" s="50" t="s">
-        <v>178</v>
-      </c>
       <c r="D10" s="51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E10" s="51"/>
       <c r="F10" s="52"/>
@@ -7974,10 +7934,10 @@
         <v>21</v>
       </c>
       <c r="B11" s="47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D11" s="48"/>
       <c r="E11" s="48"/>
@@ -8009,16 +7969,16 @@
     </row>
     <row r="12" spans="1:30" ht="19">
       <c r="A12" s="53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B12" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="53" t="s">
         <v>170</v>
       </c>
-      <c r="C12" s="53" t="s">
-        <v>171</v>
-      </c>
       <c r="D12" s="48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E12" s="48"/>
       <c r="F12" s="52"/>
@@ -8049,16 +8009,16 @@
     </row>
     <row r="13" spans="1:30" ht="38">
       <c r="A13" s="53" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B13" s="50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C13" s="53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E13" s="48"/>
       <c r="F13" s="52"/>
@@ -8092,10 +8052,10 @@
         <v>22</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C14" s="54" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D14" s="48"/>
       <c r="E14" s="48"/>
@@ -8166,7 +8126,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C16" s="42"/>
       <c r="D16" s="43"/>
@@ -8270,14 +8230,14 @@
         <v>72</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C19" s="59" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D19" s="51"/>
       <c r="E19" s="51" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F19" s="55"/>
       <c r="G19" s="55"/>
@@ -8307,13 +8267,13 @@
     </row>
     <row r="20" spans="1:30" ht="57">
       <c r="A20" s="75" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B20" s="58" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" s="59" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D20" s="51"/>
       <c r="E20" s="51"/>
@@ -8348,7 +8308,7 @@
         <v>27</v>
       </c>
       <c r="B21" s="60" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C21" s="47"/>
       <c r="D21" s="48"/>
@@ -8381,19 +8341,19 @@
     </row>
     <row r="22" spans="1:30" ht="38">
       <c r="A22" s="61" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C22" s="62" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D22" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E22" s="48" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F22" s="52"/>
       <c r="G22" s="55"/>
@@ -8423,19 +8383,19 @@
     </row>
     <row r="23" spans="1:30" ht="38">
       <c r="A23" s="61" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B23" s="61" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C23" s="62" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D23" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E23" s="48" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F23" s="52"/>
       <c r="G23" s="55"/>
@@ -8465,16 +8425,16 @@
     </row>
     <row r="24" spans="1:30" ht="38">
       <c r="A24" s="61" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B24" s="61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C24" s="62" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D24" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E24" s="48"/>
       <c r="F24" s="52"/>
@@ -8505,16 +8465,16 @@
     </row>
     <row r="25" spans="1:30" ht="38">
       <c r="A25" s="61" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B25" s="61" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C25" s="62" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D25" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E25" s="48"/>
       <c r="F25" s="52"/>
@@ -8545,16 +8505,16 @@
     </row>
     <row r="26" spans="1:30" ht="38">
       <c r="A26" s="61" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C26" s="62" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D26" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E26" s="48"/>
       <c r="F26" s="52"/>
@@ -8585,16 +8545,16 @@
     </row>
     <row r="27" spans="1:30" ht="95">
       <c r="A27" s="61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B27" s="61" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C27" s="62" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D27" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E27" s="48"/>
       <c r="F27" s="52"/>
@@ -8625,16 +8585,16 @@
     </row>
     <row r="28" spans="1:30" ht="38">
       <c r="A28" s="61" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B28" s="61" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C28" s="62" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D28" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E28" s="48"/>
       <c r="F28" s="52"/>
@@ -8665,16 +8625,16 @@
     </row>
     <row r="29" spans="1:30" ht="38">
       <c r="A29" s="61" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B29" s="61" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C29" s="62" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D29" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E29" s="48"/>
       <c r="F29" s="52"/>
@@ -8705,16 +8665,16 @@
     </row>
     <row r="30" spans="1:30" ht="76">
       <c r="A30" s="61" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B30" s="61" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C30" s="62" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D30" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E30" s="48"/>
       <c r="F30" s="52"/>
@@ -8745,16 +8705,16 @@
     </row>
     <row r="31" spans="1:30" ht="38">
       <c r="A31" s="61" t="s">
+        <v>271</v>
+      </c>
+      <c r="B31" s="61" t="s">
         <v>273</v>
       </c>
-      <c r="B31" s="61" t="s">
+      <c r="C31" s="62" t="s">
         <v>275</v>
       </c>
-      <c r="C31" s="62" t="s">
-        <v>277</v>
-      </c>
       <c r="D31" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E31" s="48"/>
       <c r="F31" s="52"/>
@@ -8785,16 +8745,16 @@
     </row>
     <row r="32" spans="1:30" ht="38">
       <c r="A32" s="61" t="s">
+        <v>272</v>
+      </c>
+      <c r="B32" s="61" t="s">
         <v>274</v>
       </c>
-      <c r="B32" s="61" t="s">
+      <c r="C32" s="62" t="s">
         <v>276</v>
       </c>
-      <c r="C32" s="62" t="s">
-        <v>278</v>
-      </c>
       <c r="D32" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E32" s="48"/>
       <c r="F32" s="52"/>
@@ -8825,16 +8785,16 @@
     </row>
     <row r="33" spans="1:30" ht="38">
       <c r="A33" s="61" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B33" s="61" t="s">
+        <v>204</v>
+      </c>
+      <c r="C33" s="62" t="s">
         <v>205</v>
       </c>
-      <c r="C33" s="62" t="s">
-        <v>206</v>
-      </c>
       <c r="D33" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E33" s="48"/>
       <c r="F33" s="52"/>
@@ -8865,16 +8825,16 @@
     </row>
     <row r="34" spans="1:30" ht="95">
       <c r="A34" s="61" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B34" s="61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C34" s="62" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E34" s="48"/>
       <c r="F34" s="52"/>
@@ -8904,15 +8864,15 @@
       <c r="AD34" s="55"/>
     </row>
     <row r="35" spans="1:30">
-      <c r="A35" s="117" t="s">
-        <v>158</v>
-      </c>
-      <c r="B35" s="117" t="s">
-        <v>249</v>
-      </c>
-      <c r="C35" s="117"/>
-      <c r="D35" s="111"/>
-      <c r="E35" s="111"/>
+      <c r="A35" s="114" t="s">
+        <v>157</v>
+      </c>
+      <c r="B35" s="114" t="s">
+        <v>248</v>
+      </c>
+      <c r="C35" s="114"/>
+      <c r="D35" s="117"/>
+      <c r="E35" s="117"/>
       <c r="F35" s="52"/>
       <c r="G35" s="55"/>
       <c r="H35" s="55"/>
@@ -8940,11 +8900,11 @@
       <c r="AD35" s="55"/>
     </row>
     <row r="36" spans="1:30">
-      <c r="A36" s="118"/>
-      <c r="B36" s="118"/>
-      <c r="C36" s="118"/>
-      <c r="D36" s="112"/>
-      <c r="E36" s="112"/>
+      <c r="A36" s="115"/>
+      <c r="B36" s="115"/>
+      <c r="C36" s="115"/>
+      <c r="D36" s="118"/>
+      <c r="E36" s="118"/>
       <c r="F36" s="52"/>
       <c r="G36" s="55"/>
       <c r="H36" s="55"/>
@@ -8972,11 +8932,11 @@
       <c r="AD36" s="55"/>
     </row>
     <row r="37" spans="1:30">
-      <c r="A37" s="119"/>
-      <c r="B37" s="119"/>
-      <c r="C37" s="119"/>
-      <c r="D37" s="113"/>
-      <c r="E37" s="113"/>
+      <c r="A37" s="116"/>
+      <c r="B37" s="116"/>
+      <c r="C37" s="116"/>
+      <c r="D37" s="119"/>
+      <c r="E37" s="119"/>
       <c r="F37" s="52"/>
       <c r="G37" s="55"/>
       <c r="H37" s="55"/>
@@ -9039,16 +8999,16 @@
     </row>
     <row r="39" spans="1:30" ht="19">
       <c r="A39" s="53" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B39" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="C39" s="53" t="s">
         <v>170</v>
       </c>
-      <c r="C39" s="53" t="s">
-        <v>171</v>
-      </c>
       <c r="D39" s="48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E39" s="48"/>
       <c r="F39" s="52"/>
@@ -9079,16 +9039,16 @@
     </row>
     <row r="40" spans="1:30" ht="38">
       <c r="A40" s="53" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B40" s="50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C40" s="53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D40" s="48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E40" s="48"/>
       <c r="F40" s="52"/>
@@ -9119,16 +9079,16 @@
     </row>
     <row r="41" spans="1:30" ht="38">
       <c r="A41" s="53" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B41" s="50" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C41" s="53" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D41" s="48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E41" s="48"/>
       <c r="F41" s="52"/>
@@ -9162,7 +9122,7 @@
         <v>29</v>
       </c>
       <c r="B42" s="54" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C42" s="54"/>
       <c r="D42" s="48"/>
@@ -9195,16 +9155,16 @@
     </row>
     <row r="43" spans="1:30" ht="38">
       <c r="A43" s="77" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B43" s="64" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C43" s="64" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D43" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E43" s="48"/>
       <c r="F43" s="68"/>
@@ -9235,16 +9195,16 @@
     </row>
     <row r="44" spans="1:30" ht="38">
       <c r="A44" s="77" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B44" s="61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C44" s="64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D44" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E44" s="48"/>
       <c r="F44" s="68"/>
@@ -9275,16 +9235,16 @@
     </row>
     <row r="45" spans="1:30" ht="38">
       <c r="A45" s="77" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B45" s="64" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C45" s="64" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D45" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E45" s="48"/>
       <c r="F45" s="68"/>
@@ -9315,16 +9275,16 @@
     </row>
     <row r="46" spans="1:30" ht="38">
       <c r="A46" s="77" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B46" s="61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C46" s="64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D46" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E46" s="48"/>
       <c r="F46" s="68"/>
@@ -9355,16 +9315,16 @@
     </row>
     <row r="47" spans="1:30" ht="76">
       <c r="A47" s="77" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B47" s="61" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C47" s="64" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D47" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E47" s="48"/>
       <c r="F47" s="68"/>
@@ -9395,16 +9355,16 @@
     </row>
     <row r="48" spans="1:30" ht="38">
       <c r="A48" s="77" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B48" s="64" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C48" s="64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D48" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E48" s="48"/>
       <c r="F48" s="68"/>
@@ -9438,13 +9398,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C49" s="64" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D49" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E49" s="48"/>
       <c r="F49" s="68"/>
@@ -9475,16 +9435,16 @@
     </row>
     <row r="50" spans="1:30" ht="76">
       <c r="A50" s="77" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="B50" s="61" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C50" s="64" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E50" s="48"/>
       <c r="F50" s="68"/>
@@ -9515,10 +9475,10 @@
     </row>
     <row r="51" spans="1:30" ht="19">
       <c r="A51" s="76" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B51" s="54" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C51" s="54"/>
       <c r="D51" s="48"/>
@@ -9551,16 +9511,16 @@
     </row>
     <row r="52" spans="1:30" ht="76">
       <c r="A52" s="77" t="s">
+        <v>220</v>
+      </c>
+      <c r="B52" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="B52" s="61" t="s">
+      <c r="C52" s="64" t="s">
         <v>222</v>
       </c>
-      <c r="C52" s="64" t="s">
-        <v>223</v>
-      </c>
       <c r="D52" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E52" s="48"/>
       <c r="F52" s="68"/>
@@ -9594,13 +9554,13 @@
         <v>50</v>
       </c>
       <c r="B53" s="61" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C53" s="64" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D53" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E53" s="48"/>
       <c r="F53" s="68"/>
@@ -9634,13 +9594,13 @@
         <v>49</v>
       </c>
       <c r="B54" s="61" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C54" s="64" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D54" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E54" s="48"/>
       <c r="F54" s="68"/>
@@ -9670,15 +9630,15 @@
       <c r="AD54" s="55"/>
     </row>
     <row r="55" spans="1:30">
-      <c r="A55" s="114" t="s">
+      <c r="A55" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="B55" s="117" t="s">
-        <v>254</v>
-      </c>
-      <c r="C55" s="117"/>
-      <c r="D55" s="111"/>
-      <c r="E55" s="111"/>
+      <c r="B55" s="114" t="s">
+        <v>253</v>
+      </c>
+      <c r="C55" s="114"/>
+      <c r="D55" s="117"/>
+      <c r="E55" s="117"/>
       <c r="F55" s="65"/>
       <c r="G55" s="55"/>
       <c r="H55" s="55"/>
@@ -9706,11 +9666,11 @@
       <c r="AD55" s="55"/>
     </row>
     <row r="56" spans="1:30">
-      <c r="A56" s="115"/>
-      <c r="B56" s="118"/>
-      <c r="C56" s="118"/>
-      <c r="D56" s="112"/>
-      <c r="E56" s="112"/>
+      <c r="A56" s="112"/>
+      <c r="B56" s="115"/>
+      <c r="C56" s="115"/>
+      <c r="D56" s="118"/>
+      <c r="E56" s="118"/>
       <c r="F56" s="55"/>
       <c r="G56" s="55"/>
       <c r="H56" s="55"/>
@@ -9738,11 +9698,11 @@
       <c r="AD56" s="55"/>
     </row>
     <row r="57" spans="1:30">
-      <c r="A57" s="115"/>
-      <c r="B57" s="118"/>
-      <c r="C57" s="118"/>
-      <c r="D57" s="112"/>
-      <c r="E57" s="112"/>
+      <c r="A57" s="112"/>
+      <c r="B57" s="115"/>
+      <c r="C57" s="115"/>
+      <c r="D57" s="118"/>
+      <c r="E57" s="118"/>
       <c r="F57" s="65"/>
       <c r="G57" s="55"/>
       <c r="H57" s="55"/>
@@ -9770,11 +9730,11 @@
       <c r="AD57" s="55"/>
     </row>
     <row r="58" spans="1:30">
-      <c r="A58" s="116"/>
-      <c r="B58" s="119"/>
-      <c r="C58" s="119"/>
-      <c r="D58" s="113"/>
-      <c r="E58" s="113"/>
+      <c r="A58" s="113"/>
+      <c r="B58" s="116"/>
+      <c r="C58" s="116"/>
+      <c r="D58" s="119"/>
+      <c r="E58" s="119"/>
       <c r="F58" s="65"/>
       <c r="G58" s="55"/>
       <c r="H58" s="55"/>
@@ -9803,16 +9763,16 @@
     </row>
     <row r="59" spans="1:30" s="7" customFormat="1" ht="76">
       <c r="A59" s="77" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B59" s="64" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C59" s="64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E59" s="48"/>
       <c r="F59" s="65"/>
@@ -9843,16 +9803,16 @@
     </row>
     <row r="60" spans="1:30" s="7" customFormat="1" ht="76">
       <c r="A60" s="77" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B60" s="64" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C60" s="64" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D60" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E60" s="48"/>
       <c r="F60" s="65"/>
@@ -9883,16 +9843,16 @@
     </row>
     <row r="61" spans="1:30" s="7" customFormat="1" ht="76">
       <c r="A61" s="77" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B61" s="64" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C61" s="64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D61" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E61" s="48"/>
       <c r="F61" s="65"/>
@@ -9923,16 +9883,16 @@
     </row>
     <row r="62" spans="1:30" s="7" customFormat="1" ht="95">
       <c r="A62" s="77" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B62" s="64" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C62" s="64" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D62" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E62" s="48"/>
       <c r="F62" s="65"/>
@@ -9963,16 +9923,16 @@
     </row>
     <row r="63" spans="1:30" s="7" customFormat="1" ht="76">
       <c r="A63" s="77" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B63" s="64" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C63" s="64" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D63" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E63" s="48"/>
       <c r="F63" s="65"/>
@@ -10003,16 +9963,16 @@
     </row>
     <row r="64" spans="1:30" s="7" customFormat="1" ht="76">
       <c r="A64" s="77" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B64" s="64" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C64" s="64" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D64" s="48" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E64" s="48"/>
       <c r="F64" s="65"/>
@@ -10042,15 +10002,15 @@
       <c r="AD64" s="55"/>
     </row>
     <row r="65" spans="1:30" s="6" customFormat="1">
-      <c r="A65" s="114" t="s">
+      <c r="A65" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="117" t="s">
-        <v>258</v>
-      </c>
-      <c r="C65" s="117"/>
-      <c r="D65" s="111"/>
-      <c r="E65" s="111"/>
+      <c r="B65" s="114" t="s">
+        <v>257</v>
+      </c>
+      <c r="C65" s="114"/>
+      <c r="D65" s="117"/>
+      <c r="E65" s="117"/>
       <c r="F65" s="65"/>
       <c r="G65" s="55"/>
       <c r="H65" s="55"/>
@@ -10078,11 +10038,11 @@
       <c r="AD65" s="55"/>
     </row>
     <row r="66" spans="1:30" s="6" customFormat="1">
-      <c r="A66" s="115"/>
-      <c r="B66" s="118"/>
-      <c r="C66" s="118"/>
-      <c r="D66" s="112"/>
-      <c r="E66" s="112"/>
+      <c r="A66" s="112"/>
+      <c r="B66" s="115"/>
+      <c r="C66" s="115"/>
+      <c r="D66" s="118"/>
+      <c r="E66" s="118"/>
       <c r="F66" s="65"/>
       <c r="G66" s="55"/>
       <c r="H66" s="55"/>
@@ -10110,11 +10070,11 @@
       <c r="AD66" s="55"/>
     </row>
     <row r="67" spans="1:30">
-      <c r="A67" s="116"/>
-      <c r="B67" s="119"/>
-      <c r="C67" s="119"/>
-      <c r="D67" s="113"/>
-      <c r="E67" s="113"/>
+      <c r="A67" s="113"/>
+      <c r="B67" s="116"/>
+      <c r="C67" s="116"/>
+      <c r="D67" s="119"/>
+      <c r="E67" s="119"/>
       <c r="F67" s="65"/>
       <c r="G67" s="55"/>
       <c r="H67" s="55"/>
@@ -10211,6 +10171,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="D55:D58"/>
+    <mergeCell ref="E55:E58"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="E35:E37"/>
     <mergeCell ref="A65:A67"/>
     <mergeCell ref="B65:B67"/>
     <mergeCell ref="C65:C67"/>
@@ -10220,12 +10186,6 @@
     <mergeCell ref="A55:A58"/>
     <mergeCell ref="B55:B58"/>
     <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="D55:D58"/>
-    <mergeCell ref="E55:E58"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10989,10 +10949,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02870A35-1204-0349-84AF-DDB2D5BE1AC0}">
-  <dimension ref="A1:AD40"/>
+  <dimension ref="A1:AD41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11167,13 +11127,9 @@
       <c r="Z2" s="81"/>
       <c r="AA2" s="81"/>
       <c r="AB2" s="81"/>
-      <c r="AC2" s="81">
-        <f>100 - SUM(D2:AB2)</f>
-        <v>13</v>
-      </c>
       <c r="AD2" s="81">
         <f>100 - SUM(E2:AC2)</f>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:30" ht="17">
@@ -11231,10 +11187,13 @@
       <c r="Z3" s="81"/>
       <c r="AA3" s="81"/>
       <c r="AB3" s="81"/>
-      <c r="AC3" s="81"/>
+      <c r="AC3" s="81">
+        <f>100 - SUM(D2:AB2)</f>
+        <v>13</v>
+      </c>
       <c r="AD3" s="81">
         <f t="shared" ref="AD3:AD40" si="0">100 - SUM(E3:AC3)</f>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:30" ht="17">
@@ -11292,13 +11251,10 @@
       <c r="Z4" s="81"/>
       <c r="AA4" s="81"/>
       <c r="AB4" s="81"/>
-      <c r="AC4" s="81">
-        <f t="shared" ref="AC4:AC12" si="1">100 - SUM(D4:AB4)</f>
-        <v>13</v>
-      </c>
+      <c r="AC4" s="81"/>
       <c r="AD4" s="81">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="17">
@@ -11356,10 +11312,13 @@
       <c r="Z5" s="81"/>
       <c r="AA5" s="81"/>
       <c r="AB5" s="81"/>
-      <c r="AC5" s="81"/>
+      <c r="AC5" s="81">
+        <f>100 - SUM(D4:AB4)</f>
+        <v>13</v>
+      </c>
       <c r="AD5" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="17">
@@ -11417,13 +11376,10 @@
       <c r="Z6" s="81"/>
       <c r="AA6" s="81"/>
       <c r="AB6" s="81"/>
-      <c r="AC6" s="81">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
+      <c r="AC6" s="81"/>
       <c r="AD6" s="81">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="17">
@@ -11481,10 +11437,13 @@
       </c>
       <c r="AA7" s="81"/>
       <c r="AB7" s="81"/>
-      <c r="AC7" s="81"/>
+      <c r="AC7" s="81">
+        <f>100 - SUM(D6:AB6)</f>
+        <v>13</v>
+      </c>
       <c r="AD7" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:30" ht="17">
@@ -11540,13 +11499,10 @@
         <v>9</v>
       </c>
       <c r="AB8" s="81"/>
-      <c r="AC8" s="81">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
+      <c r="AC8" s="81"/>
       <c r="AD8" s="81">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:30" ht="17">
@@ -11602,10 +11558,13 @@
       <c r="AB9" s="81">
         <v>9</v>
       </c>
-      <c r="AC9" s="81"/>
+      <c r="AC9" s="81">
+        <f>100 - SUM(D8:AB8)</f>
+        <v>13</v>
+      </c>
       <c r="AD9" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:30" ht="17">
@@ -11660,13 +11619,10 @@
       <c r="AA10" s="81">
         <v>9</v>
       </c>
-      <c r="AC10" s="81">
-        <f>100 - SUM(E10:AA10)</f>
-        <v>13</v>
-      </c>
+      <c r="AC10" s="81"/>
       <c r="AD10" s="81">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="17">
@@ -11722,10 +11678,13 @@
       <c r="AB11" s="81">
         <v>9</v>
       </c>
-      <c r="AC11" s="81"/>
+      <c r="AC11" s="81">
+        <f>100 - SUM(E10:AA10)</f>
+        <v>13</v>
+      </c>
       <c r="AD11" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="17">
@@ -11783,13 +11742,10 @@
         <v>9</v>
       </c>
       <c r="AB12" s="81"/>
-      <c r="AC12" s="81">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
+      <c r="AC12" s="81"/>
       <c r="AD12" s="81">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="17">
@@ -11847,10 +11803,13 @@
       </c>
       <c r="AA13" s="81"/>
       <c r="AB13" s="81"/>
-      <c r="AC13" s="81"/>
+      <c r="AC13" s="81">
+        <f>100 - SUM(D12:AB12)</f>
+        <v>13</v>
+      </c>
       <c r="AD13" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="17">
@@ -11908,13 +11867,10 @@
       <c r="Z14" s="81"/>
       <c r="AA14" s="81"/>
       <c r="AB14" s="81"/>
-      <c r="AC14" s="81">
-        <f ca="1">100 - SUM(E14:AC14)</f>
+      <c r="AC14" s="81"/>
+      <c r="AD14" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD14" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="17">
@@ -11972,10 +11928,13 @@
       <c r="Z15" s="81"/>
       <c r="AA15" s="81"/>
       <c r="AB15" s="81"/>
-      <c r="AC15" s="81"/>
+      <c r="AC15" s="81">
+        <f>100 - SUM(E14:AC14)</f>
+        <v>13</v>
+      </c>
       <c r="AD15" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="17">
@@ -12033,13 +11992,10 @@
       <c r="Z16" s="81"/>
       <c r="AA16" s="81"/>
       <c r="AB16" s="81"/>
-      <c r="AC16" s="81">
-        <f ca="1">100 - SUM(E16:AC16)</f>
+      <c r="AC16" s="81"/>
+      <c r="AD16" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD16" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="17">
@@ -12097,10 +12053,13 @@
       <c r="Z17" s="81"/>
       <c r="AA17" s="81"/>
       <c r="AB17" s="81"/>
-      <c r="AC17" s="81"/>
+      <c r="AC17" s="81">
+        <f>100 - SUM(E16:AC16)</f>
+        <v>13</v>
+      </c>
       <c r="AD17" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:30" ht="17">
@@ -12158,13 +12117,10 @@
       <c r="Z18" s="81"/>
       <c r="AA18" s="81"/>
       <c r="AB18" s="81"/>
-      <c r="AC18" s="81">
-        <f ca="1">100 - SUM(E18:AC18)</f>
+      <c r="AC18" s="81"/>
+      <c r="AD18" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD18" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:30" ht="17">
@@ -12222,10 +12178,13 @@
       <c r="Z19" s="81"/>
       <c r="AA19" s="81"/>
       <c r="AB19" s="81"/>
-      <c r="AC19" s="81"/>
+      <c r="AC19" s="81">
+        <f>100 - SUM(E18:AC18)</f>
+        <v>13</v>
+      </c>
       <c r="AD19" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:30" ht="17">
@@ -12281,13 +12240,10 @@
       <c r="Z20" s="81"/>
       <c r="AA20" s="81"/>
       <c r="AB20" s="81"/>
-      <c r="AC20" s="81">
-        <f ca="1">100 - SUM(E20:AC20)</f>
+      <c r="AC20" s="81"/>
+      <c r="AD20" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD20" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:30" ht="17">
@@ -12343,21 +12299,24 @@
       <c r="Z21" s="81"/>
       <c r="AA21" s="81"/>
       <c r="AB21" s="81"/>
-      <c r="AC21" s="81"/>
+      <c r="AC21" s="81">
+        <f>100 - SUM(E20:AC20)</f>
+        <v>13</v>
+      </c>
       <c r="AD21" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="34">
       <c r="A22" s="85" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B22" s="85" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D22" s="85"/>
       <c r="E22" s="81"/>
@@ -12402,24 +12361,21 @@
       <c r="Z22" s="81"/>
       <c r="AA22" s="81"/>
       <c r="AB22" s="81"/>
-      <c r="AC22" s="81">
-        <f ca="1">100 - SUM(E22:AC22)</f>
+      <c r="AC22" s="81"/>
+      <c r="AD22" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD22" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:30" ht="34">
       <c r="A23" s="85" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B23" s="85" t="s">
         <v>39</v>
       </c>
       <c r="C23" s="85" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D23" s="85"/>
       <c r="E23" s="81"/>
@@ -12464,21 +12420,24 @@
       <c r="Z23" s="81"/>
       <c r="AA23" s="81"/>
       <c r="AB23" s="81"/>
-      <c r="AC23" s="81"/>
+      <c r="AC23" s="81">
+        <f>100 - SUM(E22:AC22)</f>
+        <v>13</v>
+      </c>
       <c r="AD23" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="34">
       <c r="A24" s="85" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B24" s="85" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="85" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D24" s="85"/>
       <c r="E24" s="81"/>
@@ -12523,24 +12482,21 @@
       <c r="Z24" s="81"/>
       <c r="AA24" s="81"/>
       <c r="AB24" s="81"/>
-      <c r="AC24" s="81">
-        <f ca="1">100 - SUM(E24:AC24)</f>
+      <c r="AC24" s="81"/>
+      <c r="AD24" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD24" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="34">
       <c r="A25" s="85" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B25" s="85" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="85" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D25" s="85"/>
       <c r="E25" s="81"/>
@@ -12585,15 +12541,18 @@
       <c r="Z25" s="81"/>
       <c r="AA25" s="81"/>
       <c r="AB25" s="81"/>
-      <c r="AC25" s="81"/>
+      <c r="AC25" s="81">
+        <f>100 - SUM(E24:AC24)</f>
+        <v>13</v>
+      </c>
       <c r="AD25" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="17">
       <c r="A26" s="85" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B26" s="85" t="s">
         <v>40</v>
@@ -12644,18 +12603,15 @@
       <c r="Z26" s="81"/>
       <c r="AA26" s="81"/>
       <c r="AB26" s="81"/>
-      <c r="AC26" s="81">
-        <f ca="1">100 - SUM(E26:AC26)</f>
+      <c r="AC26" s="81"/>
+      <c r="AD26" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD26" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="17">
       <c r="A27" s="85" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B27" s="85" t="s">
         <v>40</v>
@@ -12706,15 +12662,18 @@
       <c r="Z27" s="81"/>
       <c r="AA27" s="81"/>
       <c r="AB27" s="81"/>
-      <c r="AC27" s="81"/>
+      <c r="AC27" s="81">
+        <f>100 - SUM(E26:AC26)</f>
+        <v>13</v>
+      </c>
       <c r="AD27" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:30" ht="17">
       <c r="A28" s="85" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B28" s="85" t="s">
         <v>40</v>
@@ -12824,13 +12783,10 @@
       <c r="Z29" s="81"/>
       <c r="AA29" s="81"/>
       <c r="AB29" s="81"/>
-      <c r="AC29" s="81">
-        <f ca="1">100 - SUM(E29:AC29)</f>
+      <c r="AC29" s="81"/>
+      <c r="AD29" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD29" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:30" ht="17">
@@ -12886,10 +12842,13 @@
       <c r="Z30" s="81"/>
       <c r="AA30" s="81"/>
       <c r="AB30" s="81"/>
-      <c r="AC30" s="81"/>
+      <c r="AC30" s="81">
+        <f>100 - SUM(E29:AC29)</f>
+        <v>13</v>
+      </c>
       <c r="AD30" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:30" ht="17">
@@ -13004,13 +12963,10 @@
       <c r="Z32" s="81"/>
       <c r="AA32" s="81"/>
       <c r="AB32" s="81"/>
-      <c r="AC32" s="81">
-        <f ca="1">100 - SUM(E32:AC32)</f>
+      <c r="AC32" s="81"/>
+      <c r="AD32" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD32" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:30" ht="17">
@@ -13066,10 +13022,13 @@
       <c r="Z33" s="81"/>
       <c r="AA33" s="81"/>
       <c r="AB33" s="81"/>
-      <c r="AC33" s="81"/>
+      <c r="AC33" s="81">
+        <f>100 - SUM(E32:AC32)</f>
+        <v>13</v>
+      </c>
       <c r="AD33" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:30" ht="17">
@@ -13125,13 +13084,10 @@
       <c r="Z34" s="81"/>
       <c r="AA34" s="81"/>
       <c r="AB34" s="81"/>
-      <c r="AC34" s="81">
-        <f ca="1">100 - SUM(E34:AC34)</f>
+      <c r="AC34" s="81"/>
+      <c r="AD34" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD34" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:30" ht="17">
@@ -13187,10 +13143,13 @@
       <c r="Z35" s="81"/>
       <c r="AA35" s="81"/>
       <c r="AB35" s="81"/>
-      <c r="AC35" s="81"/>
+      <c r="AC35" s="81">
+        <f>100 - SUM(E34:AC34)</f>
+        <v>13</v>
+      </c>
       <c r="AD35" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:30" ht="17">
@@ -13246,13 +13205,10 @@
       <c r="Z36" s="81"/>
       <c r="AA36" s="81"/>
       <c r="AB36" s="81"/>
-      <c r="AC36" s="81">
-        <f ca="1">100 - SUM(E36:AC36)</f>
+      <c r="AC36" s="81"/>
+      <c r="AD36" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD36" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:30" ht="17">
@@ -13308,10 +13264,13 @@
       <c r="Z37" s="81"/>
       <c r="AA37" s="81"/>
       <c r="AB37" s="81"/>
-      <c r="AC37" s="81"/>
+      <c r="AC37" s="81">
+        <f>100 - SUM(E36:AC36)</f>
+        <v>13</v>
+      </c>
       <c r="AD37" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="17">
@@ -13426,13 +13385,10 @@
       <c r="Z39" s="81"/>
       <c r="AA39" s="81"/>
       <c r="AB39" s="81"/>
-      <c r="AC39" s="81">
-        <f ca="1">100 - SUM(E39:AC39)</f>
+      <c r="AC39" s="81"/>
+      <c r="AD39" s="81">
+        <f t="shared" si="0"/>
         <v>13</v>
-      </c>
-      <c r="AD39" s="81">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:30" ht="17">
@@ -13488,11 +13444,17 @@
       <c r="Z40" s="81"/>
       <c r="AA40" s="81"/>
       <c r="AB40" s="81"/>
-      <c r="AC40" s="81"/>
+      <c r="AC40" s="81">
+        <f>100 - SUM(E39:AC39)</f>
+        <v>13</v>
+      </c>
       <c r="AD40" s="81">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30">
+      <c r="AC41" s="81"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -13504,8 +13466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECD6FA8-0314-8846-BFDF-FA8162BED368}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -14436,13 +14398,13 @@
     </row>
     <row r="22" spans="1:14" ht="34">
       <c r="A22" s="85" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B22" s="85" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="85" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D22" s="85"/>
       <c r="E22" s="81">
@@ -14478,13 +14440,13 @@
     </row>
     <row r="23" spans="1:14" ht="34">
       <c r="A23" s="85" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B23" s="85" t="s">
         <v>39</v>
       </c>
       <c r="C23" s="85" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D23" s="85"/>
       <c r="E23" s="81">
@@ -14520,13 +14482,13 @@
     </row>
     <row r="24" spans="1:14" ht="34">
       <c r="A24" s="85" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B24" s="85" t="s">
         <v>39</v>
       </c>
       <c r="C24" s="85" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D24" s="85"/>
       <c r="E24" s="81">
@@ -14562,13 +14524,13 @@
     </row>
     <row r="25" spans="1:14" ht="34">
       <c r="A25" s="85" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B25" s="85" t="s">
         <v>39</v>
       </c>
       <c r="C25" s="85" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D25" s="85"/>
       <c r="E25" s="81">
@@ -14604,7 +14566,7 @@
     </row>
     <row r="26" spans="1:14" ht="17">
       <c r="A26" s="85" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B26" s="85" t="s">
         <v>40</v>
@@ -14646,7 +14608,7 @@
     </row>
     <row r="27" spans="1:14" ht="17">
       <c r="A27" s="85" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B27" s="85" t="s">
         <v>40</v>
@@ -14688,7 +14650,7 @@
     </row>
     <row r="28" spans="1:14" ht="17">
       <c r="A28" s="85" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B28" s="85" t="s">
         <v>40</v>
@@ -15240,10 +15202,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860AE2CD-C5E0-9D4F-A277-50B033BCB6A0}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15261,50 +15223,36 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="17">
-      <c r="A2" s="81" t="s">
-        <v>272</v>
+    <row r="2" spans="1:8">
+      <c r="A2" s="79" t="s">
+        <v>400</v>
       </c>
       <c r="B2" s="79">
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="17">
-      <c r="A3" s="81" t="s">
-        <v>116</v>
+    <row r="3" spans="1:8">
+      <c r="A3" s="79" t="s">
+        <v>401</v>
       </c>
       <c r="B3" s="79">
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="17">
-      <c r="A4" s="81" t="s">
-        <v>150</v>
+    <row r="4" spans="1:8">
+      <c r="A4" s="79" t="s">
+        <v>402</v>
       </c>
       <c r="B4" s="79">
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="34">
-      <c r="A5" s="81" t="s">
-        <v>151</v>
-      </c>
-      <c r="B5" s="79">
-        <v>2000</v>
-      </c>
+    <row r="5" spans="1:8">
       <c r="D5" s="85"/>
       <c r="E5" s="85"/>
       <c r="F5" s="85"/>
       <c r="G5" s="85"/>
       <c r="H5" s="85"/>
-    </row>
-    <row r="6" spans="1:8" ht="17">
-      <c r="A6" s="81" t="s">
-        <v>154</v>
-      </c>
-      <c r="B6" s="79">
-        <v>1000</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -15317,7 +15265,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15337,7 +15285,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="79" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2" s="79">
         <v>30000</v>
@@ -15546,7 +15494,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -15566,7 +15514,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="86" t="s">
-        <v>208</v>
+        <v>403</v>
       </c>
       <c r="B2" s="79">
         <v>2000</v>
@@ -15574,7 +15522,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="86" t="s">
-        <v>209</v>
+        <v>290</v>
       </c>
       <c r="B3" s="79">
         <v>2000</v>

</xml_diff>

<commit_message>
feat: modify import scripts
</commit_message>
<xml_diff>
--- a/成本核算数据源配置表.xlsx
+++ b/成本核算数据源配置表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xinliao/Projects/gitclone/python-excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A497D7D8-B0E9-BD4E-BECE-37D9A28A6C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F4E1CD-08F4-294C-B0E4-B3F3E35E29A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-68960" yWindow="-840" windowWidth="28800" windowHeight="17500" xr2:uid="{97E2786A-046E-A540-BAE7-43526A264538}"/>
+    <workbookView xWindow="-68960" yWindow="-840" windowWidth="28800" windowHeight="17500" activeTab="3" xr2:uid="{97E2786A-046E-A540-BAE7-43526A264538}"/>
   </bookViews>
   <sheets>
     <sheet name="人员费用配置表" sheetId="20" r:id="rId1"/>
@@ -2603,7 +2603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CC9293E-C443-5D4F-807A-3A2F963837CD}">
   <dimension ref="A1:BO42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+    <sheetView topLeftCell="D2" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
@@ -10196,8 +10196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6662D507-57B7-FA47-A175-53794A1823B8}">
   <dimension ref="A1:AA8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>